<commit_message>
added national validity code and dataset
</commit_message>
<xml_diff>
--- a/Prelim_Data/Arizona_Alluvial/Arizona_Alluvial_30_95.xlsx
+++ b/Prelim_Data/Arizona_Alluvial/Arizona_Alluvial_30_95.xlsx
@@ -518,7 +518,7 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>inter_annual</t>
+          <t>inter_annual%</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
@@ -640,7 +640,7 @@
         <v>44104</v>
       </c>
       <c r="D2" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E2" t="n">
         <v>0.95</v>
@@ -676,7 +676,7 @@
         <v>0.228118250861872</v>
       </c>
       <c r="P2" t="n">
-        <v>0.4666666666666667</v>
+        <v>47</v>
       </c>
       <c r="Q2" t="n">
         <v>3.5</v>
@@ -761,7 +761,7 @@
         <v>44104</v>
       </c>
       <c r="D3" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E3" t="n">
         <v>0.95</v>
@@ -797,7 +797,7 @@
         <v>0.006177249764865832</v>
       </c>
       <c r="P3" t="n">
-        <v>0.8333333333333334</v>
+        <v>83</v>
       </c>
       <c r="Q3" t="n">
         <v>4.16</v>
@@ -882,7 +882,7 @@
         <v>44104</v>
       </c>
       <c r="D4" t="n">
-        <v>11.89048596851472</v>
+        <v>12</v>
       </c>
       <c r="E4" t="n">
         <v>0.95</v>
@@ -912,16 +912,16 @@
         <v>19.36363636363636</v>
       </c>
       <c r="N4" t="n">
-        <v>1.716833908812518</v>
+        <v>1.704712696691306</v>
       </c>
       <c r="O4" t="n">
-        <v>1.116757989797275e-05</v>
+        <v>1.10861200530809e-05</v>
       </c>
       <c r="P4" t="n">
-        <v>0.9166666666666666</v>
+        <v>92</v>
       </c>
       <c r="Q4" t="n">
-        <v>10.81818181818182</v>
+        <v>10.90909090909091</v>
       </c>
       <c r="R4" t="n">
         <v>239.0909090909091</v>
@@ -1003,7 +1003,7 @@
         <v>44104</v>
       </c>
       <c r="D5" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E5" t="n">
         <v>0.95</v>
@@ -1039,7 +1039,7 @@
         <v>0.0006990215684589449</v>
       </c>
       <c r="P5" t="n">
-        <v>0.6</v>
+        <v>60</v>
       </c>
       <c r="Q5" t="n">
         <v>3.388888888888889</v>
@@ -1124,7 +1124,7 @@
         <v>44104</v>
       </c>
       <c r="D6" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E6" t="n">
         <v>0.95</v>
@@ -1160,7 +1160,7 @@
         <v>0.004589499611220306</v>
       </c>
       <c r="P6" t="n">
-        <v>0.6666666666666666</v>
+        <v>67</v>
       </c>
       <c r="Q6" t="n">
         <v>3.45</v>
@@ -1245,7 +1245,7 @@
         <v>44104</v>
       </c>
       <c r="D7" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E7" t="n">
         <v>0.95</v>
@@ -1281,7 +1281,7 @@
         <v>0.004049805869244173</v>
       </c>
       <c r="P7" t="n">
-        <v>0.8333333333333334</v>
+        <v>83</v>
       </c>
       <c r="Q7" t="n">
         <v>4.12</v>
@@ -1366,7 +1366,7 @@
         <v>44104</v>
       </c>
       <c r="D8" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E8" t="n">
         <v>0.95</v>
@@ -1402,7 +1402,7 @@
         <v>0.0002537443871335606</v>
       </c>
       <c r="P8" t="n">
-        <v>0.4333333333333333</v>
+        <v>43</v>
       </c>
       <c r="Q8" t="n">
         <v>3.461538461538462</v>
@@ -1487,7 +1487,7 @@
         <v>44104</v>
       </c>
       <c r="D9" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E9" t="n">
         <v>0.95</v>
@@ -1523,7 +1523,7 @@
         <v>0.005999304252103521</v>
       </c>
       <c r="P9" t="n">
-        <v>0.8666666666666667</v>
+        <v>87</v>
       </c>
       <c r="Q9" t="n">
         <v>3.653846153846154</v>
@@ -1608,7 +1608,7 @@
         <v>44104</v>
       </c>
       <c r="D10" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E10" t="n">
         <v>0.95</v>
@@ -1644,7 +1644,7 @@
         <v>0.0006728691483456625</v>
       </c>
       <c r="P10" t="n">
-        <v>0.4666666666666667</v>
+        <v>47</v>
       </c>
       <c r="Q10" t="n">
         <v>3.142857142857143</v>
@@ -1729,7 +1729,7 @@
         <v>44104</v>
       </c>
       <c r="D11" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E11" t="n">
         <v>0.95</v>
@@ -1765,7 +1765,7 @@
         <v>0.0009702221450427252</v>
       </c>
       <c r="P11" t="n">
-        <v>0.7333333333333333</v>
+        <v>73</v>
       </c>
       <c r="Q11" t="n">
         <v>4.590909090909091</v>
@@ -1850,7 +1850,7 @@
         <v>44104</v>
       </c>
       <c r="D12" t="n">
-        <v>28.99931553730322</v>
+        <v>29</v>
       </c>
       <c r="E12" t="n">
         <v>0.95</v>
@@ -1886,7 +1886,7 @@
         <v>0.005415857148478923</v>
       </c>
       <c r="P12" t="n">
-        <v>0.896551724137931</v>
+        <v>90</v>
       </c>
       <c r="Q12" t="n">
         <v>3.884615384615385</v>
@@ -1971,7 +1971,7 @@
         <v>44104</v>
       </c>
       <c r="D13" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E13" t="n">
         <v>0.95</v>
@@ -2007,7 +2007,7 @@
         <v>0.0001491392040802542</v>
       </c>
       <c r="P13" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="Q13" t="n">
         <v>5.25</v>
@@ -2092,7 +2092,7 @@
         <v>44104</v>
       </c>
       <c r="D14" t="n">
-        <v>17.78507871321013</v>
+        <v>18</v>
       </c>
       <c r="E14" t="n">
         <v>0.95</v>
@@ -2128,7 +2128,7 @@
         <v>0.0003102551740170476</v>
       </c>
       <c r="P14" t="n">
-        <v>0.7222222222222222</v>
+        <v>72</v>
       </c>
       <c r="Q14" t="n">
         <v>3.769230769230769</v>
@@ -2213,7 +2213,7 @@
         <v>44104</v>
       </c>
       <c r="D15" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E15" t="n">
         <v>0.95</v>
@@ -2249,7 +2249,7 @@
         <v>0.003101950419418314</v>
       </c>
       <c r="P15" t="n">
-        <v>0.7666666666666667</v>
+        <v>77</v>
       </c>
       <c r="Q15" t="n">
         <v>3.478260869565217</v>
@@ -2334,7 +2334,7 @@
         <v>44104</v>
       </c>
       <c r="D16" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E16" t="n">
         <v>0.95</v>
@@ -2364,16 +2364,16 @@
         <v>21.88</v>
       </c>
       <c r="N16" t="n">
-        <v>3.371878787878788</v>
+        <v>3.351878787878788</v>
       </c>
       <c r="O16" t="n">
-        <v>0.001082682855473793</v>
+        <v>0.00108252344748487</v>
       </c>
       <c r="P16" t="n">
-        <v>0.8333333333333334</v>
+        <v>83</v>
       </c>
       <c r="Q16" t="n">
-        <v>5.6</v>
+        <v>5.64</v>
       </c>
       <c r="R16" t="n">
         <v>195.76</v>
@@ -2455,7 +2455,7 @@
         <v>44104</v>
       </c>
       <c r="D17" t="n">
-        <v>18.25051334702259</v>
+        <v>19</v>
       </c>
       <c r="E17" t="n">
         <v>0.95</v>
@@ -2491,7 +2491,7 @@
         <v>0.0008504736461985859</v>
       </c>
       <c r="P17" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="Q17" t="n">
         <v>8.631578947368421</v>
@@ -2576,7 +2576,7 @@
         <v>44104</v>
       </c>
       <c r="D18" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E18" t="n">
         <v>0.95</v>
@@ -2612,7 +2612,7 @@
         <v>0.008662411627966823</v>
       </c>
       <c r="P18" t="n">
-        <v>0.7666666666666667</v>
+        <v>77</v>
       </c>
       <c r="Q18" t="n">
         <v>6.434782608695652</v>
@@ -2697,7 +2697,7 @@
         <v>44104</v>
       </c>
       <c r="D19" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E19" t="n">
         <v>0.95</v>
@@ -2733,7 +2733,7 @@
         <v>0.01578924499348792</v>
       </c>
       <c r="P19" t="n">
-        <v>0.8333333333333334</v>
+        <v>83</v>
       </c>
       <c r="Q19" t="n">
         <v>3.64</v>
@@ -2818,7 +2818,7 @@
         <v>44104</v>
       </c>
       <c r="D20" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E20" t="n">
         <v>0.95</v>
@@ -2854,7 +2854,7 @@
         <v>0.004719938920895321</v>
       </c>
       <c r="P20" t="n">
-        <v>0.8666666666666667</v>
+        <v>87</v>
       </c>
       <c r="Q20" t="n">
         <v>3.346153846153846</v>
@@ -2939,7 +2939,7 @@
         <v>44104</v>
       </c>
       <c r="D21" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E21" t="n">
         <v>0.95</v>
@@ -2968,21 +2968,17 @@
       <c r="M21" t="n">
         <v>36.26666666666667</v>
       </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="N21" t="n">
+        <v>12.39666666666667</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.03755248805923776</v>
       </c>
       <c r="P21" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="Q21" t="n">
-        <v>2.133333333333333</v>
+        <v>2.2</v>
       </c>
       <c r="R21" t="n">
         <v>165.4</v>
@@ -3064,7 +3060,7 @@
         <v>44104</v>
       </c>
       <c r="D22" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E22" t="n">
         <v>0.95</v>
@@ -3100,7 +3096,7 @@
         <v>0.0009829565082112126</v>
       </c>
       <c r="P22" t="n">
-        <v>0.7666666666666667</v>
+        <v>77</v>
       </c>
       <c r="Q22" t="n">
         <v>5.086956521739131</v>
@@ -3185,7 +3181,7 @@
         <v>44104</v>
       </c>
       <c r="D23" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E23" t="n">
         <v>0.95</v>
@@ -3221,7 +3217,7 @@
         <v>1.4315357578639e-05</v>
       </c>
       <c r="P23" t="n">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="Q23" t="n">
         <v>13.66666666666667</v>
@@ -3306,7 +3302,7 @@
         <v>44104</v>
       </c>
       <c r="D24" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E24" t="n">
         <v>0.95</v>
@@ -3342,7 +3338,7 @@
         <v>0.0001590418149105733</v>
       </c>
       <c r="P24" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="Q24" t="n">
         <v>11</v>
@@ -3427,7 +3423,7 @@
         <v>44104</v>
       </c>
       <c r="D25" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E25" t="n">
         <v>0.95</v>
@@ -3463,7 +3459,7 @@
         <v>0.0005104896731682391</v>
       </c>
       <c r="P25" t="n">
-        <v>0.8333333333333334</v>
+        <v>83</v>
       </c>
       <c r="Q25" t="n">
         <v>7.44</v>
@@ -3548,7 +3544,7 @@
         <v>44104</v>
       </c>
       <c r="D26" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E26" t="n">
         <v>0.95</v>
@@ -3578,16 +3574,16 @@
         <v>21.95833333333333</v>
       </c>
       <c r="N26" t="n">
-        <v>2.569773860398861</v>
+        <v>2.555758708883709</v>
       </c>
       <c r="O26" t="n">
-        <v>0.006882884729039429</v>
+        <v>0.006864442739126485</v>
       </c>
       <c r="P26" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="Q26" t="n">
-        <v>6.541666666666667</v>
+        <v>6.583333333333333</v>
       </c>
       <c r="R26" t="n">
         <v>197</v>
@@ -3669,7 +3665,7 @@
         <v>44104</v>
       </c>
       <c r="D27" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E27" t="n">
         <v>0.95</v>
@@ -3699,16 +3695,16 @@
         <v>19.62962962962963</v>
       </c>
       <c r="N27" t="n">
-        <v>1.30953315538668</v>
+        <v>1.298422044275569</v>
       </c>
       <c r="O27" t="n">
-        <v>2.135339744092576e-05</v>
+        <v>2.11347460782192e-05</v>
       </c>
       <c r="P27" t="n">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="Q27" t="n">
-        <v>14.81481481481481</v>
+        <v>14.85185185185185</v>
       </c>
       <c r="R27" t="n">
         <v>216.5555555555555</v>
@@ -3790,7 +3786,7 @@
         <v>44104</v>
       </c>
       <c r="D28" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E28" t="n">
         <v>0.95</v>
@@ -3820,16 +3816,16 @@
         <v>18.81481481481481</v>
       </c>
       <c r="N28" t="n">
-        <v>1.340811264758633</v>
+        <v>1.338518495799198</v>
       </c>
       <c r="O28" t="n">
-        <v>2.816150911380186e-05</v>
+        <v>2.811352689144879e-05</v>
       </c>
       <c r="P28" t="n">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="Q28" t="n">
-        <v>11.74074074074074</v>
+        <v>11.77777777777778</v>
       </c>
       <c r="R28" t="n">
         <v>136.6666666666667</v>
@@ -3911,7 +3907,7 @@
         <v>44104</v>
       </c>
       <c r="D29" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E29" t="n">
         <v>0.95</v>
@@ -3947,7 +3943,7 @@
         <v>4.462063374168788e-05</v>
       </c>
       <c r="P29" t="n">
-        <v>0.9333333333333333</v>
+        <v>93</v>
       </c>
       <c r="Q29" t="n">
         <v>13.25</v>
@@ -4032,7 +4028,7 @@
         <v>44104</v>
       </c>
       <c r="D30" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E30" t="n">
         <v>0.95</v>
@@ -4062,16 +4058,16 @@
         <v>22.70833333333333</v>
       </c>
       <c r="N30" t="n">
-        <v>7.332291666666666</v>
+        <v>6.950347222222223</v>
       </c>
       <c r="O30" t="n">
-        <v>0.03894832736879952</v>
+        <v>0.03857335568612232</v>
       </c>
       <c r="P30" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="Q30" t="n">
-        <v>2.458333333333333</v>
+        <v>2.5</v>
       </c>
       <c r="R30" t="n">
         <v>194.5</v>
@@ -4153,7 +4149,7 @@
         <v>44104</v>
       </c>
       <c r="D31" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E31" t="n">
         <v>0.95</v>
@@ -4189,7 +4185,7 @@
         <v>0.0004464355874002938</v>
       </c>
       <c r="P31" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="Q31" t="n">
         <v>8.6</v>
@@ -4274,7 +4270,7 @@
         <v>44104</v>
       </c>
       <c r="D32" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E32" t="n">
         <v>0.95</v>
@@ -4304,16 +4300,16 @@
         <v>18.26666666666667</v>
       </c>
       <c r="N32" t="n">
-        <v>1.522902181459726</v>
+        <v>1.519634207603517</v>
       </c>
       <c r="O32" t="n">
-        <v>3.730433646276231e-05</v>
+        <v>3.720490102307798e-05</v>
       </c>
       <c r="P32" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="Q32" t="n">
-        <v>11.03333333333333</v>
+        <v>11.06666666666667</v>
       </c>
       <c r="R32" t="n">
         <v>227.3333333333333</v>
@@ -4395,7 +4391,7 @@
         <v>44104</v>
       </c>
       <c r="D33" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E33" t="n">
         <v>0.95</v>
@@ -4425,16 +4421,16 @@
         <v>17.76666666666667</v>
       </c>
       <c r="N33" t="n">
-        <v>1.454276798554292</v>
+        <v>1.449033056788811</v>
       </c>
       <c r="O33" t="n">
-        <v>1.10441144078787e-05</v>
+        <v>1.100393787449108e-05</v>
       </c>
       <c r="P33" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="Q33" t="n">
-        <v>12.13333333333333</v>
+        <v>12.2</v>
       </c>
       <c r="R33" t="n">
         <v>227</v>
@@ -4516,7 +4512,7 @@
         <v>44104</v>
       </c>
       <c r="D34" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E34" t="n">
         <v>0.95</v>
@@ -4546,16 +4542,16 @@
         <v>23.69565217391304</v>
       </c>
       <c r="N34" t="n">
-        <v>4.474037308991543</v>
+        <v>4.398554217204103</v>
       </c>
       <c r="O34" t="n">
-        <v>0.006626502084315096</v>
+        <v>0.006424511861681078</v>
       </c>
       <c r="P34" t="n">
-        <v>0.7666666666666667</v>
+        <v>77</v>
       </c>
       <c r="Q34" t="n">
-        <v>4.304347826086956</v>
+        <v>4.391304347826087</v>
       </c>
       <c r="R34" t="n">
         <v>178.4782608695652</v>
@@ -4637,7 +4633,7 @@
         <v>44104</v>
       </c>
       <c r="D35" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E35" t="n">
         <v>0.95</v>
@@ -4673,7 +4669,7 @@
         <v>1.066509134078015e-05</v>
       </c>
       <c r="P35" t="n">
-        <v>0.9666666666666667</v>
+        <v>97</v>
       </c>
       <c r="Q35" t="n">
         <v>15.41379310344828</v>
@@ -4758,7 +4754,7 @@
         <v>44104</v>
       </c>
       <c r="D36" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E36" t="n">
         <v>0.95</v>
@@ -4788,16 +4784,16 @@
         <v>19.59259259259259</v>
       </c>
       <c r="N36" t="n">
-        <v>1.522895211784101</v>
+        <v>1.51609679757828</v>
       </c>
       <c r="O36" t="n">
-        <v>2.124544047980724e-05</v>
+        <v>2.113034200647692e-05</v>
       </c>
       <c r="P36" t="n">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="Q36" t="n">
-        <v>12.62962962962963</v>
+        <v>12.7037037037037</v>
       </c>
       <c r="R36" t="n">
         <v>207.4444444444445</v>
@@ -4879,7 +4875,7 @@
         <v>44104</v>
       </c>
       <c r="D37" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E37" t="n">
         <v>0.95</v>
@@ -4915,7 +4911,7 @@
         <v>2.06942732122714e-05</v>
       </c>
       <c r="P37" t="n">
-        <v>0.9666666666666667</v>
+        <v>97</v>
       </c>
       <c r="Q37" t="n">
         <v>9.862068965517242</v>
@@ -5000,7 +4996,7 @@
         <v>44104</v>
       </c>
       <c r="D38" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E38" t="n">
         <v>0.95</v>
@@ -5030,16 +5026,16 @@
         <v>20.26923076923077</v>
       </c>
       <c r="N38" t="n">
-        <v>2.962586878933032</v>
+        <v>2.948163802009955</v>
       </c>
       <c r="O38" t="n">
-        <v>0.0009472120763878483</v>
+        <v>0.0009447027681352944</v>
       </c>
       <c r="P38" t="n">
-        <v>0.8666666666666667</v>
+        <v>87</v>
       </c>
       <c r="Q38" t="n">
-        <v>7.038461538461538</v>
+        <v>7.076923076923077</v>
       </c>
       <c r="R38" t="n">
         <v>205.6923076923077</v>
@@ -5121,7 +5117,7 @@
         <v>44104</v>
       </c>
       <c r="D39" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E39" t="n">
         <v>0.95</v>
@@ -5157,7 +5153,7 @@
         <v>0.001082975268823874</v>
       </c>
       <c r="P39" t="n">
-        <v>0.9333333333333333</v>
+        <v>93</v>
       </c>
       <c r="Q39" t="n">
         <v>5.285714285714286</v>
@@ -5242,7 +5238,7 @@
         <v>44104</v>
       </c>
       <c r="D40" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E40" t="n">
         <v>0.95</v>
@@ -5278,7 +5274,7 @@
         <v>0.000342252484287307</v>
       </c>
       <c r="P40" t="n">
-        <v>0.9666666666666667</v>
+        <v>97</v>
       </c>
       <c r="Q40" t="n">
         <v>5.620689655172414</v>
@@ -5363,7 +5359,7 @@
         <v>44104</v>
       </c>
       <c r="D41" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E41" t="n">
         <v>0.95</v>
@@ -5393,16 +5389,16 @@
         <v>22.375</v>
       </c>
       <c r="N41" t="n">
-        <v>1.331359396914929</v>
+        <v>1.330123521208714</v>
       </c>
       <c r="O41" t="n">
-        <v>7.401217124087408e-06</v>
+        <v>7.391118088728812e-06</v>
       </c>
       <c r="P41" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="Q41" t="n">
-        <v>14.08333333333333</v>
+        <v>14.125</v>
       </c>
       <c r="R41" t="n">
         <v>147.5416666666667</v>
@@ -5484,7 +5480,7 @@
         <v>44104</v>
       </c>
       <c r="D42" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E42" t="n">
         <v>0.95</v>
@@ -5520,7 +5516,7 @@
         <v>5.949872301160129e-06</v>
       </c>
       <c r="P42" t="n">
-        <v>0.6666666666666666</v>
+        <v>67</v>
       </c>
       <c r="Q42" t="n">
         <v>14.25</v>
@@ -5605,7 +5601,7 @@
         <v>44104</v>
       </c>
       <c r="D43" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E43" t="n">
         <v>0.95</v>
@@ -5641,7 +5637,7 @@
         <v>0.0001219163097679865</v>
       </c>
       <c r="P43" t="n">
-        <v>0.6333333333333333</v>
+        <v>63</v>
       </c>
       <c r="Q43" t="n">
         <v>5.368421052631579</v>
@@ -5726,7 +5722,7 @@
         <v>44104</v>
       </c>
       <c r="D44" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E44" t="n">
         <v>0.95</v>
@@ -5762,7 +5758,7 @@
         <v>1.261012262097487e-05</v>
       </c>
       <c r="P44" t="n">
-        <v>0.9333333333333333</v>
+        <v>93</v>
       </c>
       <c r="Q44" t="n">
         <v>2.714285714285714</v>
@@ -5847,7 +5843,7 @@
         <v>44104</v>
       </c>
       <c r="D45" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E45" t="n">
         <v>0.95</v>
@@ -5877,16 +5873,16 @@
         <v>23.78260869565218</v>
       </c>
       <c r="N45" t="n">
-        <v>6.210403726708074</v>
+        <v>6.172722567287785</v>
       </c>
       <c r="O45" t="n">
-        <v>0.01436561398714096</v>
+        <v>0.01430426167311691</v>
       </c>
       <c r="P45" t="n">
-        <v>0.7666666666666667</v>
+        <v>77</v>
       </c>
       <c r="Q45" t="n">
-        <v>3.695652173913043</v>
+        <v>3.739130434782609</v>
       </c>
       <c r="R45" t="n">
         <v>200.3478260869565</v>
@@ -5968,7 +5964,7 @@
         <v>44104</v>
       </c>
       <c r="D46" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E46" t="n">
         <v>0.95</v>
@@ -6004,7 +6000,7 @@
         <v>0.01535285003562739</v>
       </c>
       <c r="P46" t="n">
-        <v>0.8333333333333334</v>
+        <v>83</v>
       </c>
       <c r="Q46" t="n">
         <v>3.32</v>
@@ -6089,7 +6085,7 @@
         <v>44104</v>
       </c>
       <c r="D47" t="n">
-        <v>24.99931553730322</v>
+        <v>25</v>
       </c>
       <c r="E47" t="n">
         <v>0.95</v>
@@ -6119,16 +6115,16 @@
         <v>21.71428571428572</v>
       </c>
       <c r="N47" t="n">
-        <v>6.461791383219956</v>
+        <v>6.410204081632655</v>
       </c>
       <c r="O47" t="n">
-        <v>0.01240988885891805</v>
+        <v>0.01234099639829853</v>
       </c>
       <c r="P47" t="n">
-        <v>0.84</v>
+        <v>84</v>
       </c>
       <c r="Q47" t="n">
-        <v>3.333333333333333</v>
+        <v>3.380952380952381</v>
       </c>
       <c r="R47" t="n">
         <v>201.7142857142857</v>
@@ -6210,7 +6206,7 @@
         <v>44104</v>
       </c>
       <c r="D48" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E48" t="n">
         <v>0.95</v>
@@ -6246,7 +6242,7 @@
         <v>0.007526154863174935</v>
       </c>
       <c r="P48" t="n">
-        <v>0.7</v>
+        <v>70</v>
       </c>
       <c r="Q48" t="n">
         <v>3.619047619047619</v>
@@ -6331,7 +6327,7 @@
         <v>44104</v>
       </c>
       <c r="D49" t="n">
-        <v>22.00136892539357</v>
+        <v>23</v>
       </c>
       <c r="E49" t="n">
         <v>0.95</v>
@@ -6367,7 +6363,7 @@
         <v>0.003247037978206985</v>
       </c>
       <c r="P49" t="n">
-        <v>0.7391304347826086</v>
+        <v>74</v>
       </c>
       <c r="Q49" t="n">
         <v>4.058823529411764</v>
@@ -6452,7 +6448,7 @@
         <v>44104</v>
       </c>
       <c r="D50" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E50" t="n">
         <v>0.95</v>
@@ -6488,7 +6484,7 @@
         <v>0.01690711784918181</v>
       </c>
       <c r="P50" t="n">
-        <v>0.7333333333333333</v>
+        <v>73</v>
       </c>
       <c r="Q50" t="n">
         <v>3.727272727272727</v>
@@ -6573,7 +6569,7 @@
         <v>44104</v>
       </c>
       <c r="D51" t="n">
-        <v>2.064339493497604</v>
+        <v>3</v>
       </c>
       <c r="E51" t="n">
         <v>0.95</v>
@@ -6609,7 +6605,7 @@
         <v>0.001700088648448984</v>
       </c>
       <c r="P51" t="n">
-        <v>0.6666666666666666</v>
+        <v>67</v>
       </c>
       <c r="Q51" t="n">
         <v>4.5</v>
@@ -6694,7 +6690,7 @@
         <v>44104</v>
       </c>
       <c r="D52" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E52" t="n">
         <v>0.95</v>
@@ -6730,7 +6726,7 @@
         <v>0.008981984371564212</v>
       </c>
       <c r="P52" t="n">
-        <v>0.7</v>
+        <v>70</v>
       </c>
       <c r="Q52" t="n">
         <v>3.476190476190476</v>
@@ -6815,7 +6811,7 @@
         <v>44104</v>
       </c>
       <c r="D53" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E53" t="n">
         <v>0.95</v>
@@ -6851,7 +6847,7 @@
         <v>0.04735964257304731</v>
       </c>
       <c r="P53" t="n">
-        <v>0.7666666666666667</v>
+        <v>77</v>
       </c>
       <c r="Q53" t="n">
         <v>3.391304347826087</v>
@@ -6936,7 +6932,7 @@
         <v>44104</v>
       </c>
       <c r="D54" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E54" t="n">
         <v>0.95</v>
@@ -6972,7 +6968,7 @@
         <v>0.05595766258322005</v>
       </c>
       <c r="P54" t="n">
-        <v>0.7</v>
+        <v>70</v>
       </c>
       <c r="Q54" t="n">
         <v>2.952380952380953</v>
@@ -7057,7 +7053,7 @@
         <v>44104</v>
       </c>
       <c r="D55" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E55" t="n">
         <v>0.95</v>
@@ -7093,7 +7089,7 @@
         <v>0.007235992147622631</v>
       </c>
       <c r="P55" t="n">
-        <v>0.9333333333333333</v>
+        <v>93</v>
       </c>
       <c r="Q55" t="n">
         <v>4.178571428571429</v>
@@ -7178,7 +7174,7 @@
         <v>44104</v>
       </c>
       <c r="D56" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E56" t="n">
         <v>0.95</v>
@@ -7214,7 +7210,7 @@
         <v>0.01018174248129101</v>
       </c>
       <c r="P56" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="Q56" t="n">
         <v>4</v>
@@ -7299,7 +7295,7 @@
         <v>44104</v>
       </c>
       <c r="D57" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E57" t="n">
         <v>0.95</v>
@@ -7335,7 +7331,7 @@
         <v>0.002140674385662259</v>
       </c>
       <c r="P57" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="Q57" t="n">
         <v>4.916666666666667</v>
@@ -7420,7 +7416,7 @@
         <v>44104</v>
       </c>
       <c r="D58" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E58" t="n">
         <v>0.95</v>
@@ -7456,7 +7452,7 @@
         <v>0.09129682084608287</v>
       </c>
       <c r="P58" t="n">
-        <v>0.1666666666666667</v>
+        <v>17</v>
       </c>
       <c r="Q58" t="n">
         <v>3</v>
@@ -7541,7 +7537,7 @@
         <v>44104</v>
       </c>
       <c r="D59" t="n">
-        <v>29.96577686516085</v>
+        <v>30</v>
       </c>
       <c r="E59" t="n">
         <v>0.95</v>
@@ -7571,16 +7567,16 @@
         <v>18.72</v>
       </c>
       <c r="N59" t="n">
-        <v>2.730705627705628</v>
+        <v>2.711658008658008</v>
       </c>
       <c r="O59" t="n">
-        <v>0.002354267024323038</v>
+        <v>0.002343736963172021</v>
       </c>
       <c r="P59" t="n">
-        <v>0.8333333333333334</v>
+        <v>83</v>
       </c>
       <c r="Q59" t="n">
-        <v>6.6</v>
+        <v>6.64</v>
       </c>
       <c r="R59" t="n">
         <v>283.64</v>
@@ -7662,7 +7658,7 @@
         <v>44104</v>
       </c>
       <c r="D60" t="n">
-        <v>26.83093771389459</v>
+        <v>27</v>
       </c>
       <c r="E60" t="n">
         <v>0.95</v>
@@ -7692,16 +7688,16 @@
         <v>28.82352941176471</v>
       </c>
       <c r="N60" t="n">
-        <v>10.62549019607843</v>
+        <v>10.0078431372549</v>
       </c>
       <c r="O60" t="n">
-        <v>0.0001994617726700303</v>
+        <v>0.0001966841898440049</v>
       </c>
       <c r="P60" t="n">
-        <v>0.6296296296296297</v>
+        <v>63</v>
       </c>
       <c r="Q60" t="n">
-        <v>2.647058823529412</v>
+        <v>2.705882352941177</v>
       </c>
       <c r="R60" t="n">
         <v>251.4705882352941</v>
@@ -7783,7 +7779,7 @@
         <v>44104</v>
       </c>
       <c r="D61" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E61" t="n">
         <v>0.95</v>
@@ -7819,7 +7815,7 @@
         <v>0.002878391515765864</v>
       </c>
       <c r="P61" t="n">
-        <v>0.9666666666666667</v>
+        <v>97</v>
       </c>
       <c r="Q61" t="n">
         <v>5.793103448275862</v>
@@ -7904,7 +7900,7 @@
         <v>44104</v>
       </c>
       <c r="D62" t="n">
-        <v>24.02737850787132</v>
+        <v>25</v>
       </c>
       <c r="E62" t="n">
         <v>0.95</v>
@@ -7940,7 +7936,7 @@
         <v>0.002925895022509539</v>
       </c>
       <c r="P62" t="n">
-        <v>0.92</v>
+        <v>92</v>
       </c>
       <c r="Q62" t="n">
         <v>5.521739130434782</v>
@@ -8025,7 +8021,7 @@
         <v>44104</v>
       </c>
       <c r="D63" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E63" t="n">
         <v>0.95</v>
@@ -8061,7 +8057,7 @@
         <v>0.00176336521265288</v>
       </c>
       <c r="P63" t="n">
-        <v>0.9333333333333333</v>
+        <v>93</v>
       </c>
       <c r="Q63" t="n">
         <v>5.357142857142857</v>
@@ -8146,7 +8142,7 @@
         <v>44104</v>
       </c>
       <c r="D64" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E64" t="n">
         <v>0.95</v>
@@ -8182,7 +8178,7 @@
         <v>0.03343249852821864</v>
       </c>
       <c r="P64" t="n">
-        <v>0.4666666666666667</v>
+        <v>47</v>
       </c>
       <c r="Q64" t="n">
         <v>4.214285714285714</v>
@@ -8267,7 +8263,7 @@
         <v>44104</v>
       </c>
       <c r="D65" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E65" t="n">
         <v>0.95</v>
@@ -8303,7 +8299,7 @@
         <v>0.0003475995622778357</v>
       </c>
       <c r="P65" t="n">
-        <v>0.7</v>
+        <v>70</v>
       </c>
       <c r="Q65" t="n">
         <v>4.333333333333333</v>
@@ -8388,7 +8384,7 @@
         <v>44104</v>
       </c>
       <c r="D66" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E66" t="n">
         <v>0.95</v>
@@ -8424,7 +8420,7 @@
         <v>0.001512519992469869</v>
       </c>
       <c r="P66" t="n">
-        <v>0.9333333333333333</v>
+        <v>93</v>
       </c>
       <c r="Q66" t="n">
         <v>4.464285714285714</v>
@@ -8509,7 +8505,7 @@
         <v>44104</v>
       </c>
       <c r="D67" t="n">
-        <v>28.99931553730322</v>
+        <v>29</v>
       </c>
       <c r="E67" t="n">
         <v>0.95</v>
@@ -8545,7 +8541,7 @@
         <v>0.001124899349713581</v>
       </c>
       <c r="P67" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="Q67" t="n">
         <v>7.655172413793103</v>
@@ -8630,7 +8626,7 @@
         <v>44104</v>
       </c>
       <c r="D68" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E68" t="n">
         <v>0.95</v>
@@ -8666,7 +8662,7 @@
         <v>0.001168556987036785</v>
       </c>
       <c r="P68" t="n">
-        <v>0.9333333333333333</v>
+        <v>93</v>
       </c>
       <c r="Q68" t="n">
         <v>4.678571428571429</v>
@@ -8751,7 +8747,7 @@
         <v>44104</v>
       </c>
       <c r="D69" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E69" t="n">
         <v>0.95</v>
@@ -8787,7 +8783,7 @@
         <v>0.003287850311061246</v>
       </c>
       <c r="P69" t="n">
-        <v>0.7333333333333333</v>
+        <v>73</v>
       </c>
       <c r="Q69" t="n">
         <v>4.772727272727272</v>
@@ -8872,7 +8868,7 @@
         <v>44104</v>
       </c>
       <c r="D70" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E70" t="n">
         <v>0.95</v>
@@ -8908,7 +8904,7 @@
         <v>0.0003786467350935726</v>
       </c>
       <c r="P70" t="n">
-        <v>0.9666666666666667</v>
+        <v>97</v>
       </c>
       <c r="Q70" t="n">
         <v>7.172413793103448</v>
@@ -8993,7 +8989,7 @@
         <v>44104</v>
       </c>
       <c r="D71" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E71" t="n">
         <v>0.95</v>
@@ -9029,7 +9025,7 @@
         <v>0.0007464364154314831</v>
       </c>
       <c r="P71" t="n">
-        <v>0.7666666666666667</v>
+        <v>77</v>
       </c>
       <c r="Q71" t="n">
         <v>4.217391304347826</v>
@@ -9114,7 +9110,7 @@
         <v>44104</v>
       </c>
       <c r="D72" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E72" t="n">
         <v>0.95</v>
@@ -9150,7 +9146,7 @@
         <v>0.003173732457642638</v>
       </c>
       <c r="P72" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="Q72" t="n">
         <v>8.300000000000001</v>
@@ -9235,7 +9231,7 @@
         <v>44104</v>
       </c>
       <c r="D73" t="n">
-        <v>28.40246406570842</v>
+        <v>29</v>
       </c>
       <c r="E73" t="n">
         <v>0.95</v>
@@ -9271,7 +9267,7 @@
         <v>0.0003860024152520461</v>
       </c>
       <c r="P73" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="Q73" t="n">
         <v>9.896551724137931</v>
@@ -9356,7 +9352,7 @@
         <v>44104</v>
       </c>
       <c r="D74" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E74" t="n">
         <v>0.95</v>
@@ -9392,7 +9388,7 @@
         <v>0.0006518675095460066</v>
       </c>
       <c r="P74" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="Q74" t="n">
         <v>7.5</v>
@@ -9477,7 +9473,7 @@
         <v>44104</v>
       </c>
       <c r="D75" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E75" t="n">
         <v>0.95</v>
@@ -9513,7 +9509,7 @@
         <v>0.007580721791802679</v>
       </c>
       <c r="P75" t="n">
-        <v>0.7</v>
+        <v>70</v>
       </c>
       <c r="Q75" t="n">
         <v>3.428571428571428</v>
@@ -9598,7 +9594,7 @@
         <v>44104</v>
       </c>
       <c r="D76" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E76" t="n">
         <v>0.95</v>
@@ -9634,7 +9630,7 @@
         <v>0.01442452575418106</v>
       </c>
       <c r="P76" t="n">
-        <v>0.7333333333333333</v>
+        <v>73</v>
       </c>
       <c r="Q76" t="n">
         <v>4.181818181818182</v>
@@ -9719,7 +9715,7 @@
         <v>44104</v>
       </c>
       <c r="D77" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E77" t="n">
         <v>0.95</v>
@@ -9755,7 +9751,7 @@
         <v>0.0008706494139877713</v>
       </c>
       <c r="P77" t="n">
-        <v>0.7</v>
+        <v>70</v>
       </c>
       <c r="Q77" t="n">
         <v>2.952380952380953</v>
@@ -9840,7 +9836,7 @@
         <v>44104</v>
       </c>
       <c r="D78" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E78" t="n">
         <v>0.95</v>
@@ -9876,7 +9872,7 @@
         <v>0.003911286257513445</v>
       </c>
       <c r="P78" t="n">
-        <v>0.7333333333333333</v>
+        <v>73</v>
       </c>
       <c r="Q78" t="n">
         <v>3.454545454545455</v>
@@ -9961,7 +9957,7 @@
         <v>44104</v>
       </c>
       <c r="D79" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E79" t="n">
         <v>0.95</v>
@@ -9997,7 +9993,7 @@
         <v>0.004271762102108628</v>
       </c>
       <c r="P79" t="n">
-        <v>0.7666666666666667</v>
+        <v>77</v>
       </c>
       <c r="Q79" t="n">
         <v>4.260869565217392</v>
@@ -10082,7 +10078,7 @@
         <v>44104</v>
       </c>
       <c r="D80" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E80" t="n">
         <v>0.95</v>
@@ -10118,7 +10114,7 @@
         <v>0.02596335897586768</v>
       </c>
       <c r="P80" t="n">
-        <v>0.7666666666666667</v>
+        <v>77</v>
       </c>
       <c r="Q80" t="n">
         <v>3.652173913043478</v>
@@ -10203,7 +10199,7 @@
         <v>44104</v>
       </c>
       <c r="D81" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E81" t="n">
         <v>0.95</v>
@@ -10239,7 +10235,7 @@
         <v>0.001664899279186563</v>
       </c>
       <c r="P81" t="n">
-        <v>0.9666666666666667</v>
+        <v>97</v>
       </c>
       <c r="Q81" t="n">
         <v>5.068965517241379</v>
@@ -10324,7 +10320,7 @@
         <v>44104</v>
       </c>
       <c r="D82" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E82" t="n">
         <v>0.95</v>
@@ -10360,7 +10356,7 @@
         <v>0.00288762718900632</v>
       </c>
       <c r="P82" t="n">
-        <v>0.8333333333333334</v>
+        <v>83</v>
       </c>
       <c r="Q82" t="n">
         <v>4.08</v>
@@ -10445,7 +10441,7 @@
         <v>44104</v>
       </c>
       <c r="D83" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E83" t="n">
         <v>0.95</v>
@@ -10481,7 +10477,7 @@
         <v>0.04690018839110931</v>
       </c>
       <c r="P83" t="n">
-        <v>0.7666666666666667</v>
+        <v>77</v>
       </c>
       <c r="Q83" t="n">
         <v>3.478260869565217</v>
@@ -10566,7 +10562,7 @@
         <v>44104</v>
       </c>
       <c r="D84" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E84" t="n">
         <v>0.95</v>
@@ -10602,7 +10598,7 @@
         <v>0.01601669149966778</v>
       </c>
       <c r="P84" t="n">
-        <v>0.8666666666666667</v>
+        <v>87</v>
       </c>
       <c r="Q84" t="n">
         <v>3.923076923076923</v>
@@ -10687,7 +10683,7 @@
         <v>44104</v>
       </c>
       <c r="D85" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E85" t="n">
         <v>0.95</v>
@@ -10723,7 +10719,7 @@
         <v>0.09698330936355164</v>
       </c>
       <c r="P85" t="n">
-        <v>0.4</v>
+        <v>40</v>
       </c>
       <c r="Q85" t="n">
         <v>4.666666666666667</v>
@@ -10808,7 +10804,7 @@
         <v>44104</v>
       </c>
       <c r="D86" t="n">
-        <v>19.15947980835044</v>
+        <v>20</v>
       </c>
       <c r="E86" t="n">
         <v>0.95</v>
@@ -10844,7 +10840,7 @@
         <v>0.001761280523324082</v>
       </c>
       <c r="P86" t="n">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="Q86" t="n">
         <v>2.944444444444445</v>
@@ -10929,7 +10925,7 @@
         <v>44104</v>
       </c>
       <c r="D87" t="n">
-        <v>25.99863107460643</v>
+        <v>26</v>
       </c>
       <c r="E87" t="n">
         <v>0.95</v>
@@ -10965,7 +10961,7 @@
         <v>0.0003988831310400458</v>
       </c>
       <c r="P87" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="Q87" t="n">
         <v>6.153846153846154</v>
@@ -11050,7 +11046,7 @@
         <v>44104</v>
       </c>
       <c r="D88" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E88" t="n">
         <v>0.95</v>
@@ -11086,7 +11082,7 @@
         <v>0.002714675606569206</v>
       </c>
       <c r="P88" t="n">
-        <v>0.9666666666666667</v>
+        <v>97</v>
       </c>
       <c r="Q88" t="n">
         <v>3.827586206896552</v>
@@ -11171,7 +11167,7 @@
         <v>44104</v>
       </c>
       <c r="D89" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E89" t="n">
         <v>0.95</v>
@@ -11207,7 +11203,7 @@
         <v>0.01054938278916246</v>
       </c>
       <c r="P89" t="n">
-        <v>0.8333333333333334</v>
+        <v>83</v>
       </c>
       <c r="Q89" t="n">
         <v>3.68</v>
@@ -11292,7 +11288,7 @@
         <v>44104</v>
       </c>
       <c r="D90" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E90" t="n">
         <v>0.95</v>
@@ -11328,7 +11324,7 @@
         <v>0.004431731505649661</v>
       </c>
       <c r="P90" t="n">
-        <v>0.8666666666666667</v>
+        <v>87</v>
       </c>
       <c r="Q90" t="n">
         <v>4.730769230769231</v>
@@ -11413,7 +11409,7 @@
         <v>44104</v>
       </c>
       <c r="D91" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E91" t="n">
         <v>0.95</v>
@@ -11449,7 +11445,7 @@
         <v>0.002266125771974217</v>
       </c>
       <c r="P91" t="n">
-        <v>0.8666666666666667</v>
+        <v>87</v>
       </c>
       <c r="Q91" t="n">
         <v>4.538461538461538</v>
@@ -11534,7 +11530,7 @@
         <v>44104</v>
       </c>
       <c r="D92" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E92" t="n">
         <v>0.95</v>
@@ -11570,7 +11566,7 @@
         <v>0.002939974025107226</v>
       </c>
       <c r="P92" t="n">
-        <v>0.8666666666666667</v>
+        <v>87</v>
       </c>
       <c r="Q92" t="n">
         <v>4.961538461538462</v>
@@ -11655,7 +11651,7 @@
         <v>44104</v>
       </c>
       <c r="D93" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E93" t="n">
         <v>0.95</v>
@@ -11691,7 +11687,7 @@
         <v>0.005457780349464449</v>
       </c>
       <c r="P93" t="n">
-        <v>0.7333333333333333</v>
+        <v>73</v>
       </c>
       <c r="Q93" t="n">
         <v>4.136363636363637</v>
@@ -11776,7 +11772,7 @@
         <v>44104</v>
       </c>
       <c r="D94" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E94" t="n">
         <v>0.95</v>
@@ -11812,7 +11808,7 @@
         <v>0.02565513719355703</v>
       </c>
       <c r="P94" t="n">
-        <v>0.8333333333333334</v>
+        <v>83</v>
       </c>
       <c r="Q94" t="n">
         <v>3.68</v>
@@ -11897,7 +11893,7 @@
         <v>44104</v>
       </c>
       <c r="D95" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E95" t="n">
         <v>0.95</v>
@@ -11927,16 +11923,16 @@
         <v>41.69230769230769</v>
       </c>
       <c r="N95" t="n">
-        <v>12.53399051928464</v>
+        <v>11.91860590390002</v>
       </c>
       <c r="O95" t="n">
-        <v>8.952272172431414e-05</v>
+        <v>8.566309196835476e-05</v>
       </c>
       <c r="P95" t="n">
-        <v>0.4333333333333333</v>
+        <v>43</v>
       </c>
       <c r="Q95" t="n">
-        <v>4</v>
+        <v>4.076923076923077</v>
       </c>
       <c r="R95" t="n">
         <v>248.0769230769231</v>
@@ -12018,7 +12014,7 @@
         <v>43899</v>
       </c>
       <c r="D96" t="n">
-        <v>29.43737166324435</v>
+        <v>30</v>
       </c>
       <c r="E96" t="n">
         <v>0.95</v>
@@ -12054,7 +12050,7 @@
         <v>0.005925034539028891</v>
       </c>
       <c r="P96" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="Q96" t="n">
         <v>4.75</v>
@@ -12139,7 +12135,7 @@
         <v>44104</v>
       </c>
       <c r="D97" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E97" t="n">
         <v>0.95</v>
@@ -12175,7 +12171,7 @@
         <v>0.001461799457462613</v>
       </c>
       <c r="P97" t="n">
-        <v>0.9333333333333333</v>
+        <v>93</v>
       </c>
       <c r="Q97" t="n">
         <v>4.607142857142857</v>
@@ -12260,7 +12256,7 @@
         <v>44104</v>
       </c>
       <c r="D98" t="n">
-        <v>15.00068446269678</v>
+        <v>16</v>
       </c>
       <c r="E98" t="n">
         <v>0.95</v>
@@ -12296,7 +12292,7 @@
         <v>0.02255565956510496</v>
       </c>
       <c r="P98" t="n">
-        <v>0.875</v>
+        <v>88</v>
       </c>
       <c r="Q98" t="n">
         <v>3.571428571428572</v>
@@ -12381,7 +12377,7 @@
         <v>44104</v>
       </c>
       <c r="D99" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E99" t="n">
         <v>0.95</v>
@@ -12411,16 +12407,16 @@
         <v>34</v>
       </c>
       <c r="N99" t="n">
-        <v>8.390625</v>
+        <v>8.203125</v>
       </c>
       <c r="O99" t="n">
-        <v>0.04836106562288472</v>
+        <v>0.04829913667937052</v>
       </c>
       <c r="P99" t="n">
-        <v>0.5333333333333333</v>
+        <v>53</v>
       </c>
       <c r="Q99" t="n">
-        <v>3.375</v>
+        <v>3.4375</v>
       </c>
       <c r="R99" t="n">
         <v>139.1875</v>
@@ -12502,7 +12498,7 @@
         <v>44104</v>
       </c>
       <c r="D100" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E100" t="n">
         <v>0.95</v>
@@ -12538,7 +12534,7 @@
         <v>0.004888396992351861</v>
       </c>
       <c r="P100" t="n">
-        <v>0.8666666666666667</v>
+        <v>87</v>
       </c>
       <c r="Q100" t="n">
         <v>3.269230769230769</v>
@@ -12623,7 +12619,7 @@
         <v>44104</v>
       </c>
       <c r="D101" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E101" t="n">
         <v>0.95</v>
@@ -12659,7 +12655,7 @@
         <v>0.04824951249214637</v>
       </c>
       <c r="P101" t="n">
-        <v>0.4666666666666667</v>
+        <v>47</v>
       </c>
       <c r="Q101" t="n">
         <v>3.928571428571428</v>
@@ -12744,7 +12740,7 @@
         <v>44104</v>
       </c>
       <c r="D102" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E102" t="n">
         <v>0.95</v>
@@ -12780,7 +12776,7 @@
         <v>0.002464405473324157</v>
       </c>
       <c r="P102" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="Q102" t="n">
         <v>5.366666666666666</v>
@@ -12865,7 +12861,7 @@
         <v>44104</v>
       </c>
       <c r="D103" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E103" t="n">
         <v>0.95</v>
@@ -12901,7 +12897,7 @@
         <v>0.01056442092275315</v>
       </c>
       <c r="P103" t="n">
-        <v>0.9666666666666667</v>
+        <v>97</v>
       </c>
       <c r="Q103" t="n">
         <v>4.379310344827586</v>
@@ -12986,7 +12982,7 @@
         <v>44104</v>
       </c>
       <c r="D104" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E104" t="n">
         <v>0.95</v>
@@ -13022,7 +13018,7 @@
         <v>0.001899426971622781</v>
       </c>
       <c r="P104" t="n">
-        <v>0.8333333333333334</v>
+        <v>83</v>
       </c>
       <c r="Q104" t="n">
         <v>3.96</v>
@@ -13107,7 +13103,7 @@
         <v>44104</v>
       </c>
       <c r="D105" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E105" t="n">
         <v>0.95</v>
@@ -13143,7 +13139,7 @@
         <v>0.0002209851429684874</v>
       </c>
       <c r="P105" t="n">
-        <v>0.8666666666666667</v>
+        <v>87</v>
       </c>
       <c r="Q105" t="n">
         <v>4.884615384615385</v>
@@ -13228,7 +13224,7 @@
         <v>44104</v>
       </c>
       <c r="D106" t="n">
-        <v>29.58521560574949</v>
+        <v>30</v>
       </c>
       <c r="E106" t="n">
         <v>0.95</v>
@@ -13257,21 +13253,17 @@
       <c r="M106" t="n">
         <v>21.125</v>
       </c>
-      <c r="N106" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="O106" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="N106" t="n">
+        <v>6.393518518518519</v>
+      </c>
+      <c r="O106" t="n">
+        <v>0.006996017094491359</v>
       </c>
       <c r="P106" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="Q106" t="n">
-        <v>3.208333333333333</v>
+        <v>3.25</v>
       </c>
       <c r="R106" t="n">
         <v>206.1666666666667</v>
@@ -13353,7 +13345,7 @@
         <v>44104</v>
       </c>
       <c r="D107" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E107" t="n">
         <v>0.95</v>
@@ -13382,21 +13374,17 @@
       <c r="M107" t="n">
         <v>81</v>
       </c>
-      <c r="N107" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="O107" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="N107" t="n">
+        <v>58.41666666666666</v>
+      </c>
+      <c r="O107" t="n">
+        <v>0.4218184588121424</v>
       </c>
       <c r="P107" t="n">
-        <v>0.2</v>
+        <v>20</v>
       </c>
       <c r="Q107" t="n">
-        <v>2</v>
+        <v>2.166666666666667</v>
       </c>
       <c r="R107" t="n">
         <v>162.5</v>
@@ -13478,7 +13466,7 @@
         <v>44104</v>
       </c>
       <c r="D108" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E108" t="n">
         <v>0.95</v>
@@ -13507,21 +13495,17 @@
       <c r="M108" t="n">
         <v>78.14285714285714</v>
       </c>
-      <c r="N108" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="O108" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="N108" t="n">
+        <v>72.61904761904762</v>
+      </c>
+      <c r="O108" t="n">
+        <v>0.7730666110289665</v>
       </c>
       <c r="P108" t="n">
-        <v>0.2333333333333333</v>
+        <v>23</v>
       </c>
       <c r="Q108" t="n">
-        <v>1.142857142857143</v>
+        <v>1.285714285714286</v>
       </c>
       <c r="R108" t="n">
         <v>200.5714285714286</v>
@@ -13603,7 +13587,7 @@
         <v>44104</v>
       </c>
       <c r="D109" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E109" t="n">
         <v>0.95</v>
@@ -13633,16 +13617,16 @@
         <v>21.2</v>
       </c>
       <c r="N109" t="n">
-        <v>1.618759950951767</v>
+        <v>1.612331379523196</v>
       </c>
       <c r="O109" t="n">
-        <v>7.171115387087369e-06</v>
+        <v>7.140473775924674e-06</v>
       </c>
       <c r="P109" t="n">
-        <v>0.8333333333333334</v>
+        <v>83</v>
       </c>
       <c r="Q109" t="n">
-        <v>11.8</v>
+        <v>11.84</v>
       </c>
       <c r="R109" t="n">
         <v>136.8</v>
@@ -13724,7 +13708,7 @@
         <v>44104</v>
       </c>
       <c r="D110" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E110" t="n">
         <v>0.95</v>
@@ -13754,16 +13738,16 @@
         <v>27.89473684210526</v>
       </c>
       <c r="N110" t="n">
-        <v>1.91870412746843</v>
+        <v>1.900283074836851</v>
       </c>
       <c r="O110" t="n">
-        <v>1.144995412817681e-05</v>
+        <v>1.14090576864144e-05</v>
       </c>
       <c r="P110" t="n">
-        <v>0.6333333333333333</v>
+        <v>63</v>
       </c>
       <c r="Q110" t="n">
-        <v>10.42105263157895</v>
+        <v>10.47368421052632</v>
       </c>
       <c r="R110" t="n">
         <v>106.7894736842105</v>
@@ -13845,7 +13829,7 @@
         <v>44104</v>
       </c>
       <c r="D111" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E111" t="n">
         <v>0.95</v>
@@ -13875,16 +13859,16 @@
         <v>46.90909090909091</v>
       </c>
       <c r="N111" t="n">
-        <v>8.124690461054097</v>
+        <v>7.980834317197954</v>
       </c>
       <c r="O111" t="n">
-        <v>0.0003099353942317742</v>
+        <v>0.000303465778376732</v>
       </c>
       <c r="P111" t="n">
-        <v>0.3666666666666666</v>
+        <v>37</v>
       </c>
       <c r="Q111" t="n">
-        <v>4.818181818181818</v>
+        <v>4.909090909090909</v>
       </c>
       <c r="R111" t="n">
         <v>112.3636363636364</v>
@@ -13966,7 +13950,7 @@
         <v>44104</v>
       </c>
       <c r="D112" t="n">
-        <v>29.99863107460643</v>
+        <v>30</v>
       </c>
       <c r="E112" t="n">
         <v>0.95</v>
@@ -13996,16 +13980,16 @@
         <v>25.4</v>
       </c>
       <c r="N112" t="n">
-        <v>6.449954212454213</v>
+        <v>6.424404761904762</v>
       </c>
       <c r="O112" t="n">
-        <v>0.0002318154123681724</v>
+        <v>0.000231235291666535</v>
       </c>
       <c r="P112" t="n">
-        <v>0.6666666666666666</v>
+        <v>67</v>
       </c>
       <c r="Q112" t="n">
-        <v>3.7</v>
+        <v>3.75</v>
       </c>
       <c r="R112" t="n">
         <v>253.75</v>
@@ -14087,7 +14071,7 @@
         <v>44104</v>
       </c>
       <c r="D113" t="n">
-        <v>17.91649555099247</v>
+        <v>18</v>
       </c>
       <c r="E113" t="n">
         <v>0.95</v>
@@ -14123,7 +14107,7 @@
         <v>0.0004658032789847645</v>
       </c>
       <c r="P113" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="Q113" t="n">
         <v>6.888888888888889</v>
@@ -21867,10 +21851,10 @@
         <v>165</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0584045584045584</v>
+        <v>0.05643738977072313</v>
       </c>
       <c r="J4" t="n">
-        <v>1.422262922262922</v>
+        <v>1.432098765432098</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -22632,19 +22616,19 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0.9625431107168481</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>0.04696250562296544</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.003333333333333334</v>
+        <v>0.01</v>
       </c>
       <c r="G16" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="H16" t="n">
-        <v>1811</v>
+        <v>1813.666666666667</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -22661,25 +22645,25 @@
         <v>0</v>
       </c>
       <c r="M16" t="n">
-        <v>0.4191617037357411</v>
+        <v>0.3792332644420184</v>
       </c>
       <c r="N16" t="n">
-        <v>0.8078764600676355</v>
+        <v>0.8793099093621357</v>
       </c>
       <c r="O16" t="n">
-        <v>0.1057471264367816</v>
+        <v>0.1149425287356322</v>
       </c>
       <c r="P16" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="Q16" t="n">
-        <v>3102.666666666667</v>
+        <v>3105.333333333333</v>
       </c>
       <c r="R16" t="n">
-        <v>0.04133333333333333</v>
+        <v>0.04166666666666674</v>
       </c>
       <c r="S16" t="n">
-        <v>1.817333333333334</v>
+        <v>1.812499999999999</v>
       </c>
     </row>
     <row r="17">
@@ -22957,25 +22941,25 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3464949929037819</v>
+        <v>0.6556471855286778</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.9414096057649476</v>
+        <v>-0.4459308658886594</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.1904761904761905</v>
+        <v>-0.09523809523809523</v>
       </c>
       <c r="G21" t="n">
-        <v>-20</v>
+        <v>-10</v>
       </c>
       <c r="H21" t="n">
         <v>407.3333333333333</v>
       </c>
       <c r="I21" t="n">
-        <v>-0.6071428571428571</v>
+        <v>-0.4166666666666667</v>
       </c>
       <c r="J21" t="n">
-        <v>16.25</v>
+        <v>13.91666666666667</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -22986,16 +22970,16 @@
         <v>0</v>
       </c>
       <c r="M21" t="n">
-        <v>0.08511080829021078</v>
+        <v>0.1259018931093008</v>
       </c>
       <c r="N21" t="n">
-        <v>-1.72177211239669</v>
+        <v>-1.530464099908169</v>
       </c>
       <c r="O21" t="n">
-        <v>-0.2091954022988506</v>
+        <v>-0.1862068965517241</v>
       </c>
       <c r="P21" t="n">
-        <v>-91</v>
+        <v>-81</v>
       </c>
       <c r="Q21" t="n">
         <v>2732.333333333333</v>
@@ -23347,25 +23331,25 @@
         <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>0.00262919583908916</v>
+        <v>0.004497973837224611</v>
       </c>
       <c r="E27" t="n">
-        <v>-3.008061894914459</v>
+        <v>-2.840947345196989</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.4131054131054131</v>
+        <v>-0.3903133903133903</v>
       </c>
       <c r="G27" t="n">
-        <v>-145</v>
+        <v>-137</v>
       </c>
       <c r="H27" t="n">
         <v>2291.666666666667</v>
       </c>
       <c r="I27" t="n">
-        <v>-0.02059496567505721</v>
+        <v>-0.01739130434782608</v>
       </c>
       <c r="J27" t="n">
-        <v>1.455234553775744</v>
+        <v>1.413586956521739</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
@@ -23376,25 +23360,25 @@
         <v>1</v>
       </c>
       <c r="M27" t="n">
-        <v>0.0006385014942318357</v>
+        <v>0.001069087338063213</v>
       </c>
       <c r="N27" t="n">
-        <v>-3.414709160867649</v>
+        <v>-3.271684693396753</v>
       </c>
       <c r="O27" t="n">
-        <v>-0.4413793103448276</v>
+        <v>-0.4229885057471264</v>
       </c>
       <c r="P27" t="n">
-        <v>-192</v>
+        <v>-184</v>
       </c>
       <c r="Q27" t="n">
         <v>3128.666666666667</v>
       </c>
       <c r="R27" t="n">
-        <v>-0.02380952380952381</v>
+        <v>-0.02255639097744363</v>
       </c>
       <c r="S27" t="n">
-        <v>1.481884057971015</v>
+        <v>1.463713631905852</v>
       </c>
     </row>
     <row r="28">
@@ -23412,25 +23396,25 @@
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>0.05016175000277556</v>
+        <v>0.07343753136517983</v>
       </c>
       <c r="E28" t="n">
-        <v>-1.958582079231839</v>
+        <v>-1.790101900373186</v>
       </c>
       <c r="F28" t="n">
-        <v>-0.2678062678062678</v>
+        <v>-0.245014245014245</v>
       </c>
       <c r="G28" t="n">
-        <v>-94</v>
+        <v>-86</v>
       </c>
       <c r="H28" t="n">
         <v>2254.666666666667</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.01587301587301587</v>
+        <v>-0.01484848484848489</v>
       </c>
       <c r="J28" t="n">
-        <v>1.469507101086048</v>
+        <v>1.443030303030304</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
@@ -23441,16 +23425,16 @@
         <v>1</v>
       </c>
       <c r="M28" t="n">
-        <v>0.007773825008267954</v>
+        <v>0.01180699976112298</v>
       </c>
       <c r="N28" t="n">
-        <v>-2.661738483026002</v>
+        <v>-2.517860727186759</v>
       </c>
       <c r="O28" t="n">
-        <v>-0.3425287356321839</v>
+        <v>-0.3241379310344827</v>
       </c>
       <c r="P28" t="n">
-        <v>-149</v>
+        <v>-141</v>
       </c>
       <c r="Q28" t="n">
         <v>3091.666666666667</v>
@@ -23459,7 +23443,7 @@
         <v>-0.02272727272727273</v>
       </c>
       <c r="S28" t="n">
-        <v>1.579545454545455</v>
+        <v>1.573593073593074</v>
       </c>
     </row>
     <row r="29">
@@ -23542,25 +23526,25 @@
         <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>0.02983407194339605</v>
+        <v>0.0338084650225583</v>
       </c>
       <c r="E30" t="n">
-        <v>-2.172286337059312</v>
+        <v>-2.12234872011542</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.3188405797101449</v>
+        <v>-0.3115942028985507</v>
       </c>
       <c r="G30" t="n">
-        <v>-88</v>
+        <v>-86</v>
       </c>
       <c r="H30" t="n">
         <v>1604</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.2416666666666667</v>
+        <v>-0.2277777777777778</v>
       </c>
       <c r="J30" t="n">
-        <v>5.445833333333334</v>
+        <v>5.286111111111111</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
@@ -23571,25 +23555,25 @@
         <v>0</v>
       </c>
       <c r="M30" t="n">
-        <v>0.135528499820478</v>
+        <v>0.1452036967203116</v>
       </c>
       <c r="N30" t="n">
-        <v>-1.492651252626133</v>
+        <v>-1.456683752562853</v>
       </c>
       <c r="O30" t="n">
-        <v>-0.1931034482758621</v>
+        <v>-0.1885057471264368</v>
       </c>
       <c r="P30" t="n">
-        <v>-84</v>
+        <v>-82</v>
       </c>
       <c r="Q30" t="n">
         <v>3092</v>
       </c>
       <c r="R30" t="n">
-        <v>-0.1</v>
+        <v>-0.09523809523809525</v>
       </c>
       <c r="S30" t="n">
-        <v>3.45</v>
+        <v>3.380952380952381</v>
       </c>
     </row>
     <row r="31">
@@ -23672,25 +23656,25 @@
         <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>1.548609165169523e-05</v>
+        <v>2.305505725619383e-05</v>
       </c>
       <c r="E32" t="n">
-        <v>-4.321658257499128</v>
+        <v>-4.233042834368797</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.5586206896551724</v>
+        <v>-0.5471264367816092</v>
       </c>
       <c r="G32" t="n">
-        <v>-243</v>
+        <v>-238</v>
       </c>
       <c r="H32" t="n">
-        <v>3135.666666666667</v>
+        <v>3134.666666666667</v>
       </c>
       <c r="I32" t="n">
-        <v>-0.02777777777777778</v>
+        <v>-0.02650103519668737</v>
       </c>
       <c r="J32" t="n">
-        <v>1.888071895424837</v>
+        <v>1.869559127999026</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -23701,25 +23685,25 @@
         <v>1</v>
       </c>
       <c r="M32" t="n">
-        <v>1.548609165169523e-05</v>
+        <v>2.305505725619383e-05</v>
       </c>
       <c r="N32" t="n">
-        <v>-4.321658257499128</v>
+        <v>-4.233042834368797</v>
       </c>
       <c r="O32" t="n">
-        <v>-0.5586206896551724</v>
+        <v>-0.5471264367816092</v>
       </c>
       <c r="P32" t="n">
-        <v>-243</v>
+        <v>-238</v>
       </c>
       <c r="Q32" t="n">
-        <v>3135.666666666667</v>
+        <v>3134.666666666667</v>
       </c>
       <c r="R32" t="n">
-        <v>-0.02777777777777778</v>
+        <v>-0.02650103519668737</v>
       </c>
       <c r="S32" t="n">
-        <v>1.888071895424837</v>
+        <v>1.869559127999026</v>
       </c>
     </row>
     <row r="33">
@@ -23752,10 +23736,10 @@
         <v>3135.666666666667</v>
       </c>
       <c r="I33" t="n">
-        <v>-0.01758241758241759</v>
+        <v>-0.01764705882352941</v>
       </c>
       <c r="J33" t="n">
-        <v>1.642445054945055</v>
+        <v>1.643382352941176</v>
       </c>
       <c r="K33" t="inlineStr">
         <is>
@@ -23781,10 +23765,10 @@
         <v>3135.666666666667</v>
       </c>
       <c r="R33" t="n">
-        <v>-0.01758241758241759</v>
+        <v>-0.01764705882352941</v>
       </c>
       <c r="S33" t="n">
-        <v>1.642445054945055</v>
+        <v>1.643382352941176</v>
       </c>
     </row>
     <row r="34">
@@ -23802,25 +23786,25 @@
         <v>1</v>
       </c>
       <c r="D34" t="n">
-        <v>0.005788110544914016</v>
+        <v>0.004914001595228035</v>
       </c>
       <c r="E34" t="n">
-        <v>-2.759549568869208</v>
+        <v>-2.812617829809001</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.4150197628458498</v>
+        <v>-0.4229249011857708</v>
       </c>
       <c r="G34" t="n">
-        <v>-105</v>
+        <v>-107</v>
       </c>
       <c r="H34" t="n">
         <v>1420.333333333333</v>
       </c>
       <c r="I34" t="n">
-        <v>-0.2076023391812866</v>
+        <v>-0.2045454545454546</v>
       </c>
       <c r="J34" t="n">
-        <v>4.283625730994152</v>
+        <v>4.25</v>
       </c>
       <c r="K34" t="inlineStr">
         <is>
@@ -23831,16 +23815,16 @@
         <v>1</v>
       </c>
       <c r="M34" t="n">
-        <v>0.01002373039748528</v>
+        <v>0.00902716317343466</v>
       </c>
       <c r="N34" t="n">
-        <v>-2.575009601684591</v>
+        <v>-2.611023721987872</v>
       </c>
       <c r="O34" t="n">
-        <v>-0.3310344827586207</v>
+        <v>-0.335632183908046</v>
       </c>
       <c r="P34" t="n">
-        <v>-144</v>
+        <v>-146</v>
       </c>
       <c r="Q34" t="n">
         <v>3084</v>
@@ -23932,25 +23916,25 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0.1559504396032783</v>
+        <v>0.1957921088084666</v>
       </c>
       <c r="E36" t="n">
-        <v>-1.418823637283203</v>
+        <v>-1.29363331634645</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.1965811965811966</v>
+        <v>-0.1794871794871795</v>
       </c>
       <c r="G36" t="n">
-        <v>-69</v>
+        <v>-63</v>
       </c>
       <c r="H36" t="n">
         <v>2297</v>
       </c>
       <c r="I36" t="n">
-        <v>-0.01120448179271709</v>
+        <v>-0.01071428571428572</v>
       </c>
       <c r="J36" t="n">
-        <v>1.645658263305322</v>
+        <v>1.639285714285714</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
@@ -23961,25 +23945,25 @@
         <v>1</v>
       </c>
       <c r="M36" t="n">
-        <v>0.02329383895493664</v>
+        <v>0.03066417481808492</v>
       </c>
       <c r="N36" t="n">
-        <v>-2.26858065767627</v>
+        <v>-2.161403618730934</v>
       </c>
       <c r="O36" t="n">
-        <v>-0.2942528735632184</v>
+        <v>-0.2804597701149426</v>
       </c>
       <c r="P36" t="n">
-        <v>-128</v>
+        <v>-122</v>
       </c>
       <c r="Q36" t="n">
         <v>3134</v>
       </c>
       <c r="R36" t="n">
-        <v>-0.01875</v>
+        <v>-0.01699346405228757</v>
       </c>
       <c r="S36" t="n">
-        <v>1.737242965367966</v>
+        <v>1.711773194126135</v>
       </c>
     </row>
     <row r="37">
@@ -24062,25 +24046,25 @@
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>0.4666736871765029</v>
+        <v>0.4938295761264468</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.7279018229808192</v>
+        <v>-0.6842305782761631</v>
       </c>
       <c r="F38" t="n">
-        <v>-0.1046153846153846</v>
+        <v>-0.09846153846153846</v>
       </c>
       <c r="G38" t="n">
-        <v>-34</v>
+        <v>-32</v>
       </c>
       <c r="H38" t="n">
-        <v>2055.333333333333</v>
+        <v>2052.666666666667</v>
       </c>
       <c r="I38" t="n">
-        <v>-0.02222222222222223</v>
+        <v>-0.01754385964912282</v>
       </c>
       <c r="J38" t="n">
-        <v>2.786111111111111</v>
+        <v>2.727631578947368</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
@@ -24091,19 +24075,19 @@
         <v>0</v>
       </c>
       <c r="M38" t="n">
-        <v>0.9857391711478938</v>
+        <v>0.9572175192704051</v>
       </c>
       <c r="N38" t="n">
-        <v>0.01787425013507906</v>
+        <v>0.05364560750363465</v>
       </c>
       <c r="O38" t="n">
-        <v>0.004597701149425287</v>
+        <v>0.009195402298850575</v>
       </c>
       <c r="P38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q38" t="n">
-        <v>3130</v>
+        <v>3127.333333333333</v>
       </c>
       <c r="R38" t="n">
         <v>0</v>
@@ -24257,19 +24241,19 @@
         <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>0.00890769997382157</v>
+        <v>0.01105578123133255</v>
       </c>
       <c r="E41" t="n">
-        <v>-2.615576365104856</v>
+        <v>-2.540930757404469</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.3804347826086957</v>
+        <v>-0.3695652173913043</v>
       </c>
       <c r="G41" t="n">
-        <v>-105</v>
+        <v>-102</v>
       </c>
       <c r="H41" t="n">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="I41" t="n">
         <v>-0.02222222222222222</v>
@@ -24286,25 +24270,25 @@
         <v>1</v>
       </c>
       <c r="M41" t="n">
-        <v>0.004343691433475794</v>
+        <v>0.005136238332951404</v>
       </c>
       <c r="N41" t="n">
-        <v>-2.85205990165578</v>
+        <v>-2.798362810612211</v>
       </c>
       <c r="O41" t="n">
-        <v>-0.3655172413793104</v>
+        <v>-0.3586206896551724</v>
       </c>
       <c r="P41" t="n">
-        <v>-159</v>
+        <v>-156</v>
       </c>
       <c r="Q41" t="n">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="R41" t="n">
-        <v>-0.01991769547325102</v>
+        <v>-0.01984126984126983</v>
       </c>
       <c r="S41" t="n">
-        <v>1.479715675271231</v>
+        <v>1.478607503607503</v>
       </c>
     </row>
     <row r="42">
@@ -24517,25 +24501,25 @@
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>0.1244262052652232</v>
+        <v>0.1005029674872926</v>
       </c>
       <c r="E45" t="n">
-        <v>-1.536457534195451</v>
+        <v>-1.642420122760655</v>
       </c>
       <c r="F45" t="n">
-        <v>-0.233201581027668</v>
+        <v>-0.2490118577075099</v>
       </c>
       <c r="G45" t="n">
-        <v>-59</v>
+        <v>-63</v>
       </c>
       <c r="H45" t="n">
         <v>1425</v>
       </c>
       <c r="I45" t="n">
-        <v>-0.1388888888888889</v>
+        <v>-0.15</v>
       </c>
       <c r="J45" t="n">
-        <v>6.027777777777778</v>
+        <v>5.983333333333333</v>
       </c>
       <c r="K45" t="inlineStr">
         <is>
@@ -24546,25 +24530,25 @@
         <v>0</v>
       </c>
       <c r="M45" t="n">
-        <v>0.1771735738294904</v>
+        <v>0.1551764868573369</v>
       </c>
       <c r="N45" t="n">
-        <v>-1.349508868141732</v>
+        <v>-1.421482674442625</v>
       </c>
       <c r="O45" t="n">
-        <v>-0.1747126436781609</v>
+        <v>-0.1839080459770115</v>
       </c>
       <c r="P45" t="n">
-        <v>-76</v>
+        <v>-80</v>
       </c>
       <c r="Q45" t="n">
         <v>3088.666666666667</v>
       </c>
       <c r="R45" t="n">
-        <v>-0.1</v>
+        <v>-0.1057692307692308</v>
       </c>
       <c r="S45" t="n">
-        <v>4.45</v>
+        <v>4.533653846153846</v>
       </c>
     </row>
     <row r="46">
@@ -24647,25 +24631,25 @@
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>0.716709679456915</v>
+        <v>0.856030183840685</v>
       </c>
       <c r="E47" t="n">
-        <v>0.3628597175795041</v>
+        <v>0.181429858789752</v>
       </c>
       <c r="F47" t="n">
-        <v>0.06190476190476191</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="G47" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H47" t="n">
         <v>1093.666666666667</v>
       </c>
       <c r="I47" t="n">
-        <v>0.06547619047619044</v>
+        <v>0.0326923076923077</v>
       </c>
       <c r="J47" t="n">
-        <v>4.145238095238096</v>
+        <v>4.473076923076923</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
@@ -24676,25 +24660,25 @@
         <v>0</v>
       </c>
       <c r="M47" t="n">
-        <v>0.7785910317534543</v>
+        <v>0.888203473751102</v>
       </c>
       <c r="N47" t="n">
-        <v>0.2811556337571997</v>
+        <v>0.1405778168785999</v>
       </c>
       <c r="O47" t="n">
-        <v>0.04333333333333333</v>
+        <v>0.02333333333333333</v>
       </c>
       <c r="P47" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q47" t="n">
         <v>1821.666666666667</v>
       </c>
       <c r="R47" t="n">
-        <v>0.02475490196078432</v>
+        <v>0</v>
       </c>
       <c r="S47" t="n">
-        <v>3.702941176470588</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="48">
@@ -25427,25 +25411,25 @@
         <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>0.9813092749123027</v>
+        <v>0.8698314593210195</v>
       </c>
       <c r="E59" t="n">
-        <v>-0.02342749283250609</v>
+        <v>-0.1638725722897188</v>
       </c>
       <c r="F59" t="n">
-        <v>-0.006666666666666667</v>
+        <v>-0.02666666666666667</v>
       </c>
       <c r="G59" t="n">
-        <v>-2</v>
+        <v>-8</v>
       </c>
       <c r="H59" t="n">
-        <v>1822</v>
+        <v>1824.666666666667</v>
       </c>
       <c r="I59" t="n">
-        <v>0</v>
+        <v>-0.004444444444444444</v>
       </c>
       <c r="J59" t="n">
-        <v>2.5</v>
+        <v>2.553333333333333</v>
       </c>
       <c r="K59" t="inlineStr">
         <is>
@@ -25456,25 +25440,25 @@
         <v>0</v>
       </c>
       <c r="M59" t="n">
-        <v>0.6267866347166771</v>
+        <v>0.7237813770139765</v>
       </c>
       <c r="N59" t="n">
-        <v>0.4862546410727888</v>
+        <v>0.3534096170967861</v>
       </c>
       <c r="O59" t="n">
-        <v>0.07076923076923076</v>
+        <v>0.05230769230769231</v>
       </c>
       <c r="P59" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="Q59" t="n">
-        <v>2047</v>
+        <v>2049.666666666667</v>
       </c>
       <c r="R59" t="n">
-        <v>0.01363636363636363</v>
+        <v>0.01333333333333332</v>
       </c>
       <c r="S59" t="n">
-        <v>2.279545454545455</v>
+        <v>2.283333333333334</v>
       </c>
     </row>
     <row r="60">
@@ -25492,25 +25476,25 @@
         <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>0.741535244360739</v>
+        <v>0.4580284620802866</v>
       </c>
       <c r="E60" t="n">
-        <v>-0.3298209661140196</v>
+        <v>-0.742097173756544</v>
       </c>
       <c r="F60" t="n">
-        <v>-0.06617647058823529</v>
+        <v>-0.1397058823529412</v>
       </c>
       <c r="G60" t="n">
-        <v>-9</v>
+        <v>-19</v>
       </c>
       <c r="H60" t="n">
         <v>588.3333333333334</v>
       </c>
       <c r="I60" t="n">
-        <v>-0.1277777777777778</v>
+        <v>-0.219047619047619</v>
       </c>
       <c r="J60" t="n">
-        <v>11.62222222222222</v>
+        <v>12.25238095238095</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
@@ -25521,16 +25505,16 @@
         <v>0</v>
       </c>
       <c r="M60" t="n">
-        <v>0.7315412774712367</v>
+        <v>0.8976318278433146</v>
       </c>
       <c r="N60" t="n">
-        <v>0.3430760111480943</v>
+        <v>0.1286535041805354</v>
       </c>
       <c r="O60" t="n">
-        <v>0.04843304843304843</v>
+        <v>0.01994301994301994</v>
       </c>
       <c r="P60" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="Q60" t="n">
         <v>2175</v>
@@ -28027,25 +28011,25 @@
         <v>0</v>
       </c>
       <c r="D99" t="n">
-        <v>0.3434374357957224</v>
+        <v>0.2994454590067814</v>
       </c>
       <c r="E99" t="n">
-        <v>-0.9473952006498569</v>
+        <v>-1.037623314997462</v>
       </c>
       <c r="F99" t="n">
-        <v>-0.1833333333333333</v>
+        <v>-0.2</v>
       </c>
       <c r="G99" t="n">
-        <v>-22</v>
+        <v>-24</v>
       </c>
       <c r="H99" t="n">
         <v>491.3333333333333</v>
       </c>
       <c r="I99" t="n">
-        <v>-0.1666666666666667</v>
+        <v>-0.2051282051282051</v>
       </c>
       <c r="J99" t="n">
-        <v>8.5</v>
+        <v>8.788461538461538</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -28056,16 +28040,16 @@
         <v>0</v>
       </c>
       <c r="M99" t="n">
-        <v>0.1801352971560812</v>
+        <v>0.1681740866865067</v>
       </c>
       <c r="N99" t="n">
-        <v>-1.340338570646587</v>
+        <v>-1.378094586721139</v>
       </c>
       <c r="O99" t="n">
-        <v>-0.1655172413793103</v>
+        <v>-0.1701149425287356</v>
       </c>
       <c r="P99" t="n">
-        <v>-72</v>
+        <v>-74</v>
       </c>
       <c r="Q99" t="n">
         <v>2806</v>
@@ -28475,32 +28459,32 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>decreasing</t>
+          <t>no trend</t>
         </is>
       </c>
       <c r="C106" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D106" t="n">
-        <v>0.01413409854629455</v>
+        <v>0.1072659517344385</v>
       </c>
       <c r="E106" t="n">
-        <v>-2.453837120597058</v>
+        <v>-1.610604503006401</v>
       </c>
       <c r="F106" t="n">
-        <v>-0.358695652173913</v>
+        <v>-0.2355072463768116</v>
       </c>
       <c r="G106" t="n">
-        <v>-99</v>
+        <v>-65</v>
       </c>
       <c r="H106" t="n">
-        <v>1595</v>
+        <v>1579</v>
       </c>
       <c r="I106" t="n">
-        <v>-0.1886574074074074</v>
+        <v>-0.09545454545454546</v>
       </c>
       <c r="J106" t="n">
-        <v>5.169560185185185</v>
+        <v>3.847727272727273</v>
       </c>
       <c r="K106" t="inlineStr">
         <is>
@@ -28511,25 +28495,25 @@
         <v>0</v>
       </c>
       <c r="M106" t="n">
-        <v>0.1303207261709043</v>
+        <v>0.3666082536071913</v>
       </c>
       <c r="N106" t="n">
-        <v>-1.512838344728831</v>
+        <v>-0.9028448318226533</v>
       </c>
       <c r="O106" t="n">
-        <v>-0.1954022988505747</v>
+        <v>-0.1172413793103448</v>
       </c>
       <c r="P106" t="n">
-        <v>-85</v>
+        <v>-51</v>
       </c>
       <c r="Q106" t="n">
-        <v>3083</v>
+        <v>3067</v>
       </c>
       <c r="R106" t="n">
-        <v>-0.1111111111111111</v>
+        <v>-0.03571428571428571</v>
       </c>
       <c r="S106" t="n">
-        <v>3.777777777777778</v>
+        <v>2.517857142857143</v>
       </c>
     </row>
     <row r="107">
@@ -28562,10 +28546,10 @@
         <v>27.33333333333333</v>
       </c>
       <c r="I107" t="n">
-        <v>-10.5</v>
+        <v>-1.75</v>
       </c>
       <c r="J107" t="n">
-        <v>98.25</v>
+        <v>54.875</v>
       </c>
       <c r="K107" t="inlineStr">
         <is>
@@ -28627,10 +28611,10 @@
         <v>44.33333333333334</v>
       </c>
       <c r="I108" t="n">
-        <v>-26</v>
+        <v>-10.75</v>
       </c>
       <c r="J108" t="n">
-        <v>120</v>
+        <v>74.25</v>
       </c>
       <c r="K108" t="inlineStr">
         <is>
@@ -28677,25 +28661,25 @@
         <v>0</v>
       </c>
       <c r="D109" t="n">
-        <v>0.8879383421338334</v>
+        <v>0.7780762929746678</v>
       </c>
       <c r="E109" t="n">
-        <v>0.1409134176903062</v>
+        <v>0.2818268353806125</v>
       </c>
       <c r="F109" t="n">
-        <v>0.02333333333333333</v>
+        <v>0.04333333333333333</v>
       </c>
       <c r="G109" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H109" t="n">
         <v>1813</v>
       </c>
       <c r="I109" t="n">
-        <v>0</v>
+        <v>0.001785714285714287</v>
       </c>
       <c r="J109" t="n">
-        <v>1.333333333333333</v>
+        <v>1.311904761904762</v>
       </c>
       <c r="K109" t="inlineStr">
         <is>
@@ -28706,25 +28690,25 @@
         <v>0</v>
       </c>
       <c r="M109" t="n">
-        <v>0.3600350171331905</v>
+        <v>0.3063170535701334</v>
       </c>
       <c r="N109" t="n">
-        <v>0.9152983651645634</v>
+        <v>1.022980525772159</v>
       </c>
       <c r="O109" t="n">
-        <v>0.1195402298850575</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="P109" t="n">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="Q109" t="n">
         <v>3104.666666666667</v>
       </c>
       <c r="R109" t="n">
-        <v>0.01011029411764706</v>
+        <v>0.01118012422360248</v>
       </c>
       <c r="S109" t="n">
-        <v>1.170067401960784</v>
+        <v>1.154554865424431</v>
       </c>
     </row>
     <row r="110">
@@ -28742,25 +28726,25 @@
         <v>0</v>
       </c>
       <c r="D110" t="n">
-        <v>0.313473817886444</v>
+        <v>0.2209706965420999</v>
       </c>
       <c r="E110" t="n">
-        <v>1.007959682419039</v>
+        <v>1.223951042937404</v>
       </c>
       <c r="F110" t="n">
-        <v>0.1695906432748538</v>
+        <v>0.2046783625730994</v>
       </c>
       <c r="G110" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H110" t="n">
         <v>771.6666666666666</v>
       </c>
       <c r="I110" t="n">
-        <v>0.0432900432900433</v>
+        <v>0.05000000000000004</v>
       </c>
       <c r="J110" t="n">
-        <v>1.11038961038961</v>
+        <v>1.05</v>
       </c>
       <c r="K110" t="inlineStr">
         <is>
@@ -28771,16 +28755,16 @@
         <v>0</v>
       </c>
       <c r="M110" t="n">
-        <v>0.5179874851597133</v>
+        <v>0.4488875966737558</v>
       </c>
       <c r="N110" t="n">
-        <v>0.6464507461554302</v>
+        <v>0.7572708740677896</v>
       </c>
       <c r="O110" t="n">
-        <v>0.08275862068965517</v>
+        <v>0.09655172413793103</v>
       </c>
       <c r="P110" t="n">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="Q110" t="n">
         <v>2931.333333333333</v>
@@ -30028,10 +30012,10 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1872245856104455</v>
+        <v>0.1868983086646399</v>
       </c>
       <c r="E16" t="n">
-        <v>1.318834087356051</v>
+        <v>1.319810459199841</v>
       </c>
       <c r="F16" t="n">
         <v>0.19</v>
@@ -30040,13 +30024,13 @@
         <v>57</v>
       </c>
       <c r="H16" t="n">
-        <v>1803</v>
+        <v>1800.333333333333</v>
       </c>
       <c r="I16" t="n">
-        <v>0.1602564102564102</v>
+        <v>0.1538461538461539</v>
       </c>
       <c r="J16" t="n">
-        <v>2.076923076923077</v>
+        <v>2.153846153846154</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
@@ -30057,10 +30041,10 @@
         <v>0</v>
       </c>
       <c r="M16" t="n">
-        <v>0.06409362914084005</v>
+        <v>0.06397898801642876</v>
       </c>
       <c r="N16" t="n">
-        <v>1.851528008768837</v>
+        <v>1.852326253258936</v>
       </c>
       <c r="O16" t="n">
         <v>0.2390804597701149</v>
@@ -30069,7 +30053,7 @@
         <v>104</v>
       </c>
       <c r="Q16" t="n">
-        <v>3094.666666666667</v>
+        <v>3092</v>
       </c>
       <c r="R16" t="n">
         <v>0.1666666666666667</v>
@@ -30353,19 +30337,19 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5400380006757208</v>
+        <v>0.5727314379697375</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.6127555276542502</v>
+        <v>-0.5640333466372089</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.1208791208791209</v>
+        <v>-0.1047619047619048</v>
       </c>
       <c r="G21" t="n">
         <v>-11</v>
       </c>
       <c r="H21" t="n">
-        <v>266.3333333333333</v>
+        <v>314.3333333333333</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
@@ -30382,25 +30366,25 @@
         <v>0</v>
       </c>
       <c r="M21" t="n">
-        <v>0.2535984274700616</v>
+        <v>0.1148739060726052</v>
       </c>
       <c r="N21" t="n">
-        <v>-1.141652655809487</v>
+        <v>-1.576659447659005</v>
       </c>
       <c r="O21" t="n">
-        <v>-0.135632183908046</v>
+        <v>-0.1885057471264368</v>
       </c>
       <c r="P21" t="n">
-        <v>-59</v>
+        <v>-82</v>
       </c>
       <c r="Q21" t="n">
-        <v>2581</v>
+        <v>2639.333333333333</v>
       </c>
       <c r="R21" t="n">
         <v>0</v>
       </c>
       <c r="S21" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22">
@@ -30693,10 +30677,10 @@
         <v>1604.666666666667</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.3484848484848485</v>
+        <v>-0.375</v>
       </c>
       <c r="J26" t="n">
-        <v>9.007575757575758</v>
+        <v>9.3125</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
@@ -30743,19 +30727,19 @@
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>0.9833060033679206</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>-0.02092434876593436</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.002849002849002849</v>
+        <v>-0.005698005698005698</v>
       </c>
       <c r="G27" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="H27" t="n">
-        <v>2285</v>
+        <v>2284</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
@@ -30772,25 +30756,25 @@
         <v>0</v>
       </c>
       <c r="M27" t="n">
-        <v>0.4002552721411816</v>
+        <v>0.3902300909671572</v>
       </c>
       <c r="N27" t="n">
-        <v>-0.8411654158883443</v>
+        <v>-0.859200167544049</v>
       </c>
       <c r="O27" t="n">
-        <v>-0.1103448275862069</v>
+        <v>-0.1126436781609195</v>
       </c>
       <c r="P27" t="n">
-        <v>-48</v>
+        <v>-49</v>
       </c>
       <c r="Q27" t="n">
-        <v>3122</v>
+        <v>3121</v>
       </c>
       <c r="R27" t="n">
-        <v>-0.1538461538461539</v>
+        <v>-0.1666666666666667</v>
       </c>
       <c r="S27" t="n">
-        <v>16.23076923076923</v>
+        <v>16.41666666666667</v>
       </c>
     </row>
     <row r="28">
@@ -30823,10 +30807,10 @@
         <v>2277.666666666667</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.7368421052631579</v>
+        <v>-0.7619047619047619</v>
       </c>
       <c r="J28" t="n">
-        <v>16.57894736842105</v>
+        <v>16.90476190476191</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
@@ -30852,10 +30836,10 @@
         <v>3114.666666666667</v>
       </c>
       <c r="R28" t="n">
-        <v>-0.6875</v>
+        <v>-0.7142857142857143</v>
       </c>
       <c r="S28" t="n">
-        <v>16.46875</v>
+        <v>16.85714285714286</v>
       </c>
     </row>
     <row r="29">
@@ -30938,25 +30922,25 @@
         <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>0.01751948753764898</v>
+        <v>0.009919736370315624</v>
       </c>
       <c r="E30" t="n">
-        <v>-2.375620151464374</v>
+        <v>-2.578614692299585</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.3333333333333333</v>
+        <v>-0.3623188405797101</v>
       </c>
       <c r="G30" t="n">
-        <v>-92</v>
+        <v>-100</v>
       </c>
       <c r="H30" t="n">
-        <v>1467.333333333333</v>
+        <v>1474</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.08012820512820512</v>
+        <v>-0.1</v>
       </c>
       <c r="J30" t="n">
-        <v>2.921474358974359</v>
+        <v>3.15</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
@@ -30967,25 +30951,25 @@
         <v>0</v>
       </c>
       <c r="M30" t="n">
-        <v>0.1095201089686553</v>
+        <v>0.08089002634317999</v>
       </c>
       <c r="N30" t="n">
-        <v>-1.600353840864927</v>
+        <v>-1.745545115864739</v>
       </c>
       <c r="O30" t="n">
-        <v>-0.2022988505747126</v>
+        <v>-0.2206896551724138</v>
       </c>
       <c r="P30" t="n">
-        <v>-88</v>
+        <v>-96</v>
       </c>
       <c r="Q30" t="n">
-        <v>2955.333333333333</v>
+        <v>2962</v>
       </c>
       <c r="R30" t="n">
-        <v>-0.04761904761904762</v>
+        <v>-0.0625</v>
       </c>
       <c r="S30" t="n">
-        <v>1.69047619047619</v>
+        <v>1.90625</v>
       </c>
     </row>
     <row r="31">
@@ -31068,25 +31052,25 @@
         <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>1.790795869371919e-06</v>
+        <v>1.512742451081905e-06</v>
       </c>
       <c r="E32" t="n">
-        <v>-4.775704064007028</v>
+        <v>-4.809544991719612</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.6137931034482759</v>
+        <v>-0.6183908045977011</v>
       </c>
       <c r="G32" t="n">
-        <v>-267</v>
+        <v>-269</v>
       </c>
       <c r="H32" t="n">
-        <v>3102.333333333333</v>
+        <v>3105</v>
       </c>
       <c r="I32" t="n">
-        <v>-0.55</v>
+        <v>-0.5555555555555556</v>
       </c>
       <c r="J32" t="n">
-        <v>16.475</v>
+        <v>16.55555555555556</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -31097,25 +31081,25 @@
         <v>1</v>
       </c>
       <c r="M32" t="n">
-        <v>1.790795869371919e-06</v>
+        <v>1.512742451081905e-06</v>
       </c>
       <c r="N32" t="n">
-        <v>-4.775704064007028</v>
+        <v>-4.809544991719612</v>
       </c>
       <c r="O32" t="n">
-        <v>-0.6137931034482759</v>
+        <v>-0.6183908045977011</v>
       </c>
       <c r="P32" t="n">
-        <v>-267</v>
+        <v>-269</v>
       </c>
       <c r="Q32" t="n">
-        <v>3102.333333333333</v>
+        <v>3105</v>
       </c>
       <c r="R32" t="n">
-        <v>-0.55</v>
+        <v>-0.5555555555555556</v>
       </c>
       <c r="S32" t="n">
-        <v>16.475</v>
+        <v>16.55555555555556</v>
       </c>
     </row>
     <row r="33">
@@ -31133,10 +31117,10 @@
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>0.289397861747583</v>
+        <v>0.2890866672641068</v>
       </c>
       <c r="E33" t="n">
-        <v>-1.059443469146147</v>
+        <v>-1.060127348810143</v>
       </c>
       <c r="F33" t="n">
         <v>-0.1379310344827586</v>
@@ -31145,7 +31129,7 @@
         <v>-60</v>
       </c>
       <c r="H33" t="n">
-        <v>3101.333333333333</v>
+        <v>3097.333333333333</v>
       </c>
       <c r="I33" t="n">
         <v>-0.09090909090909091</v>
@@ -31162,10 +31146,10 @@
         <v>0</v>
       </c>
       <c r="M33" t="n">
-        <v>0.289397861747583</v>
+        <v>0.2890866672641068</v>
       </c>
       <c r="N33" t="n">
-        <v>-1.059443469146147</v>
+        <v>-1.060127348810143</v>
       </c>
       <c r="O33" t="n">
         <v>-0.1379310344827586</v>
@@ -31174,7 +31158,7 @@
         <v>-60</v>
       </c>
       <c r="Q33" t="n">
-        <v>3101.333333333333</v>
+        <v>3097.333333333333</v>
       </c>
       <c r="R33" t="n">
         <v>-0.09090909090909091</v>
@@ -31242,10 +31226,10 @@
         <v>3044</v>
       </c>
       <c r="R34" t="n">
-        <v>-0.1</v>
+        <v>-0.1052631578947368</v>
       </c>
       <c r="S34" t="n">
-        <v>3.45</v>
+        <v>3.526315789473684</v>
       </c>
     </row>
     <row r="35">
@@ -31328,25 +31312,25 @@
         <v>1</v>
       </c>
       <c r="D36" t="n">
-        <v>0.0003723295295119389</v>
+        <v>0.0002911086340462443</v>
       </c>
       <c r="E36" t="n">
-        <v>-3.558957669487897</v>
+        <v>-3.623086306723166</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.4871794871794872</v>
+        <v>-0.4957264957264957</v>
       </c>
       <c r="G36" t="n">
-        <v>-171</v>
+        <v>-174</v>
       </c>
       <c r="H36" t="n">
-        <v>2281.666666666667</v>
+        <v>2280</v>
       </c>
       <c r="I36" t="n">
-        <v>-0.5</v>
+        <v>-0.52</v>
       </c>
       <c r="J36" t="n">
-        <v>18.5</v>
+        <v>18.76</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
@@ -31357,25 +31341,25 @@
         <v>1</v>
       </c>
       <c r="M36" t="n">
-        <v>4.120198569279587e-05</v>
+        <v>3.246272500811997e-05</v>
       </c>
       <c r="N36" t="n">
-        <v>-4.100633951343039</v>
+        <v>-4.155464569409333</v>
       </c>
       <c r="O36" t="n">
-        <v>-0.5287356321839081</v>
+        <v>-0.535632183908046</v>
       </c>
       <c r="P36" t="n">
-        <v>-230</v>
+        <v>-233</v>
       </c>
       <c r="Q36" t="n">
-        <v>3118.666666666667</v>
+        <v>3117</v>
       </c>
       <c r="R36" t="n">
-        <v>-0.55</v>
+        <v>-0.5714285714285714</v>
       </c>
       <c r="S36" t="n">
-        <v>18.975</v>
+        <v>19.28571428571428</v>
       </c>
     </row>
     <row r="37">
@@ -31458,16 +31442,16 @@
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>0.6240627763111095</v>
+        <v>0.6559252830194415</v>
       </c>
       <c r="E38" t="n">
-        <v>0.4901005112895243</v>
+        <v>0.445545919354113</v>
       </c>
       <c r="F38" t="n">
-        <v>0.07076923076923076</v>
+        <v>0.06461538461538462</v>
       </c>
       <c r="G38" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H38" t="n">
         <v>2015</v>
@@ -31487,16 +31471,16 @@
         <v>0</v>
       </c>
       <c r="M38" t="n">
-        <v>0.2967393299116976</v>
+        <v>0.313708866444377</v>
       </c>
       <c r="N38" t="n">
-        <v>1.043451288895128</v>
+        <v>1.00747020996771</v>
       </c>
       <c r="O38" t="n">
-        <v>0.135632183908046</v>
+        <v>0.1310344827586207</v>
       </c>
       <c r="P38" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Q38" t="n">
         <v>3089.666666666667</v>
@@ -31913,25 +31897,25 @@
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>0.08571107437880099</v>
+        <v>0.09060246700291108</v>
       </c>
       <c r="E45" t="n">
-        <v>-1.718469163331375</v>
+        <v>-1.692228224453299</v>
       </c>
       <c r="F45" t="n">
-        <v>-0.2569169960474308</v>
+        <v>-0.2529644268774703</v>
       </c>
       <c r="G45" t="n">
-        <v>-65</v>
+        <v>-64</v>
       </c>
       <c r="H45" t="n">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="I45" t="n">
-        <v>-0.1538461538461539</v>
+        <v>-0.1428571428571428</v>
       </c>
       <c r="J45" t="n">
-        <v>4.692307692307693</v>
+        <v>4.571428571428571</v>
       </c>
       <c r="K45" t="inlineStr">
         <is>
@@ -31942,25 +31926,25 @@
         <v>0</v>
       </c>
       <c r="M45" t="n">
-        <v>0.1425069980464815</v>
+        <v>0.147435042960151</v>
       </c>
       <c r="N45" t="n">
-        <v>-1.46651881936525</v>
+        <v>-1.448651100105592</v>
       </c>
       <c r="O45" t="n">
-        <v>-0.1885057471264368</v>
+        <v>-0.1862068965517241</v>
       </c>
       <c r="P45" t="n">
-        <v>-82</v>
+        <v>-81</v>
       </c>
       <c r="Q45" t="n">
-        <v>3050.666666666667</v>
+        <v>3049.666666666667</v>
       </c>
       <c r="R45" t="n">
-        <v>-0.07142857142857142</v>
+        <v>-0.06666666666666667</v>
       </c>
       <c r="S45" t="n">
-        <v>3.035714285714286</v>
+        <v>2.966666666666667</v>
       </c>
     </row>
     <row r="46">
@@ -32043,25 +32027,25 @@
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>0.1732031678481643</v>
+        <v>0.2281657092269569</v>
       </c>
       <c r="E47" t="n">
-        <v>-1.361983260934624</v>
+        <v>-1.205097384941512</v>
       </c>
       <c r="F47" t="n">
-        <v>-0.2142857142857143</v>
+        <v>-0.1904761904761905</v>
       </c>
       <c r="G47" t="n">
-        <v>-45</v>
+        <v>-40</v>
       </c>
       <c r="H47" t="n">
-        <v>1043.666666666667</v>
+        <v>1047.333333333333</v>
       </c>
       <c r="I47" t="n">
-        <v>-0.08012820512820512</v>
+        <v>-0.07417582417582418</v>
       </c>
       <c r="J47" t="n">
-        <v>3.801282051282051</v>
+        <v>3.741758241758242</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
@@ -32072,25 +32056,25 @@
         <v>0</v>
       </c>
       <c r="M47" t="n">
-        <v>0.2958612968182392</v>
+        <v>0.3546524447899291</v>
       </c>
       <c r="N47" t="n">
-        <v>-1.045349869638373</v>
+        <v>-0.925602786411397</v>
       </c>
       <c r="O47" t="n">
-        <v>-0.15</v>
+        <v>-0.1333333333333333</v>
       </c>
       <c r="P47" t="n">
-        <v>-45</v>
+        <v>-40</v>
       </c>
       <c r="Q47" t="n">
-        <v>1771.666666666667</v>
+        <v>1775.333333333333</v>
       </c>
       <c r="R47" t="n">
-        <v>-0.05882352941176471</v>
+        <v>-0.05409356725146199</v>
       </c>
       <c r="S47" t="n">
-        <v>3.705882352941177</v>
+        <v>3.649122807017544</v>
       </c>
     </row>
     <row r="48">
@@ -32823,25 +32807,25 @@
         <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>0.4101746007958811</v>
+        <v>0.3967116947961018</v>
       </c>
       <c r="E59" t="n">
-        <v>0.8235864093362705</v>
+        <v>0.8475086014221768</v>
       </c>
       <c r="F59" t="n">
-        <v>0.12</v>
+        <v>0.1233333333333333</v>
       </c>
       <c r="G59" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H59" t="n">
-        <v>1806</v>
+        <v>1804.333333333333</v>
       </c>
       <c r="I59" t="n">
-        <v>0.07692307692307693</v>
+        <v>0.08712121212121213</v>
       </c>
       <c r="J59" t="n">
-        <v>5.076923076923077</v>
+        <v>5.954545454545455</v>
       </c>
       <c r="K59" t="inlineStr">
         <is>
@@ -32852,25 +32836,25 @@
         <v>0</v>
       </c>
       <c r="M59" t="n">
-        <v>0.1830697939667474</v>
+        <v>0.1757020867933012</v>
       </c>
       <c r="N59" t="n">
-        <v>1.331362403455687</v>
+        <v>1.354107490536262</v>
       </c>
       <c r="O59" t="n">
-        <v>0.1876923076923077</v>
+        <v>0.1907692307692308</v>
       </c>
       <c r="P59" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q59" t="n">
-        <v>2031</v>
+        <v>2029.333333333333</v>
       </c>
       <c r="R59" t="n">
-        <v>0.1304347826086956</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="S59" t="n">
-        <v>4.369565217391305</v>
+        <v>4.833333333333333</v>
       </c>
     </row>
     <row r="60">
@@ -32888,25 +32872,25 @@
         <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>0.1993205477509923</v>
+        <v>0.2464412221220496</v>
       </c>
       <c r="E60" t="n">
-        <v>-1.283489751672352</v>
+        <v>-1.159036709240089</v>
       </c>
       <c r="F60" t="n">
-        <v>-0.2279411764705882</v>
+        <v>-0.2058823529411765</v>
       </c>
       <c r="G60" t="n">
-        <v>-31</v>
+        <v>-28</v>
       </c>
       <c r="H60" t="n">
-        <v>546.3333333333334</v>
+        <v>542.6666666666666</v>
       </c>
       <c r="I60" t="n">
-        <v>-0.08712121212121213</v>
+        <v>-0.03846153846153846</v>
       </c>
       <c r="J60" t="n">
-        <v>2.696969696969697</v>
+        <v>2.307692307692307</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
@@ -32917,19 +32901,19 @@
         <v>0</v>
       </c>
       <c r="M60" t="n">
-        <v>0.9309820677906129</v>
+        <v>0.9827104279740764</v>
       </c>
       <c r="N60" t="n">
-        <v>-0.08660930699488413</v>
+        <v>-0.02167096115300214</v>
       </c>
       <c r="O60" t="n">
-        <v>-0.01424501424501425</v>
+        <v>-0.005698005698005698</v>
       </c>
       <c r="P60" t="n">
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="Q60" t="n">
-        <v>2133</v>
+        <v>2129.333333333333</v>
       </c>
       <c r="R60" t="n">
         <v>0</v>
@@ -35163,25 +35147,25 @@
         <v>0</v>
       </c>
       <c r="D95" t="n">
-        <v>0.1817790633794591</v>
+        <v>0.3453414913095221</v>
       </c>
       <c r="E95" t="n">
-        <v>-1.335297295707787</v>
+        <v>-0.9436637744775487</v>
       </c>
       <c r="F95" t="n">
-        <v>-0.282051282051282</v>
+        <v>-0.2051282051282051</v>
       </c>
       <c r="G95" t="n">
-        <v>-22</v>
+        <v>-16</v>
       </c>
       <c r="H95" t="n">
-        <v>247.3333333333333</v>
+        <v>252.6666666666667</v>
       </c>
       <c r="I95" t="n">
-        <v>-0.1666666666666667</v>
+        <v>-0.1388888888888889</v>
       </c>
       <c r="J95" t="n">
-        <v>4</v>
+        <v>3.833333333333333</v>
       </c>
       <c r="K95" t="inlineStr">
         <is>
@@ -35192,25 +35176,25 @@
         <v>1</v>
       </c>
       <c r="M95" t="n">
-        <v>8.296352915482252e-05</v>
+        <v>5.10709066956494e-05</v>
       </c>
       <c r="N95" t="n">
-        <v>3.935673999470317</v>
+        <v>4.050671298463448</v>
       </c>
       <c r="O95" t="n">
-        <v>0.4574712643678161</v>
+        <v>0.4712643678160919</v>
       </c>
       <c r="P95" t="n">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="Q95" t="n">
-        <v>2531</v>
+        <v>2536.333333333333</v>
       </c>
       <c r="R95" t="n">
-        <v>0.05882352941176471</v>
+        <v>0.0625</v>
       </c>
       <c r="S95" t="n">
-        <v>-0.8529411764705882</v>
+        <v>-0.90625</v>
       </c>
     </row>
     <row r="96">
@@ -35423,10 +35407,10 @@
         <v>0</v>
       </c>
       <c r="D99" t="n">
-        <v>0.3814845914682532</v>
+        <v>0.3834953623718707</v>
       </c>
       <c r="E99" t="n">
-        <v>-0.875164159181731</v>
+        <v>-0.8714740619623809</v>
       </c>
       <c r="F99" t="n">
         <v>-0.1666666666666667</v>
@@ -35435,13 +35419,13 @@
         <v>-20</v>
       </c>
       <c r="H99" t="n">
-        <v>471.3333333333333</v>
+        <v>475.3333333333333</v>
       </c>
       <c r="I99" t="n">
-        <v>-0.08333333333333333</v>
+        <v>-0.09166666666666667</v>
       </c>
       <c r="J99" t="n">
-        <v>3.625</v>
+        <v>3.6875</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -35452,10 +35436,10 @@
         <v>0</v>
       </c>
       <c r="M99" t="n">
-        <v>0.191127937680341</v>
+        <v>0.1914464035705081</v>
       </c>
       <c r="N99" t="n">
-        <v>-1.307249651410436</v>
+        <v>-1.306312218768249</v>
       </c>
       <c r="O99" t="n">
         <v>-0.1609195402298851</v>
@@ -35464,7 +35448,7 @@
         <v>-70</v>
       </c>
       <c r="Q99" t="n">
-        <v>2786</v>
+        <v>2790</v>
       </c>
       <c r="R99" t="n">
         <v>0</v>
@@ -35878,25 +35862,25 @@
         <v>0</v>
       </c>
       <c r="D106" t="n">
-        <v>0.8496367231459785</v>
+        <v>0.8187962970278728</v>
       </c>
       <c r="E106" t="n">
-        <v>-0.1895819619409994</v>
+        <v>0.2290934335503668</v>
       </c>
       <c r="F106" t="n">
-        <v>-0.03162055335968379</v>
+        <v>0.03623188405797102</v>
       </c>
       <c r="G106" t="n">
-        <v>-8</v>
+        <v>10</v>
       </c>
       <c r="H106" t="n">
-        <v>1363.333333333333</v>
+        <v>1543.333333333333</v>
       </c>
       <c r="I106" t="n">
         <v>0</v>
       </c>
       <c r="J106" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="K106" t="inlineStr">
         <is>
@@ -35907,19 +35891,19 @@
         <v>0</v>
       </c>
       <c r="M106" t="n">
-        <v>0.5365901295868483</v>
+        <v>0.6761337586571436</v>
       </c>
       <c r="N106" t="n">
-        <v>0.6179775618345336</v>
+        <v>0.4177447382953291</v>
       </c>
       <c r="O106" t="n">
-        <v>0.08045977011494253</v>
+        <v>0.05517241379310345</v>
       </c>
       <c r="P106" t="n">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q106" t="n">
-        <v>3027</v>
+        <v>3031.333333333333</v>
       </c>
       <c r="R106" t="n">
         <v>0</v>
@@ -35949,13 +35933,13 @@
         <v>0</v>
       </c>
       <c r="F107" t="n">
-        <v>0.1</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="G107" t="n">
         <v>1</v>
       </c>
       <c r="H107" t="n">
-        <v>13</v>
+        <v>19.66666666666667</v>
       </c>
       <c r="I107" t="n">
         <v>0</v>
@@ -35965,26 +35949,26 @@
       </c>
       <c r="K107" t="inlineStr">
         <is>
-          <t>no trend</t>
+          <t>decreasing</t>
         </is>
       </c>
       <c r="L107" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M107" t="n">
-        <v>0.08112808296470608</v>
+        <v>0.02676984877830413</v>
       </c>
       <c r="N107" t="n">
-        <v>-1.7441778469463</v>
+        <v>-2.214857474544304</v>
       </c>
       <c r="O107" t="n">
-        <v>-0.1471264367816092</v>
+        <v>-0.2</v>
       </c>
       <c r="P107" t="n">
-        <v>-64</v>
+        <v>-87</v>
       </c>
       <c r="Q107" t="n">
-        <v>1304.666666666667</v>
+        <v>1507.666666666667</v>
       </c>
       <c r="R107" t="n">
         <v>0</v>
@@ -36008,19 +35992,19 @@
         <v>0</v>
       </c>
       <c r="D108" t="n">
-        <v>0.5581846494226572</v>
+        <v>0.4532547047537365</v>
       </c>
       <c r="E108" t="n">
-        <v>0.5855400437691199</v>
+        <v>0.75</v>
       </c>
       <c r="F108" t="n">
-        <v>0.2</v>
+        <v>0.1904761904761905</v>
       </c>
       <c r="G108" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H108" t="n">
-        <v>11.66666666666667</v>
+        <v>16</v>
       </c>
       <c r="I108" t="n">
         <v>0</v>
@@ -36037,19 +36021,19 @@
         <v>1</v>
       </c>
       <c r="M108" t="n">
-        <v>0.04399114775062518</v>
+        <v>0.01468757671437859</v>
       </c>
       <c r="N108" t="n">
-        <v>-2.014175149701274</v>
+        <v>-2.439992257103523</v>
       </c>
       <c r="O108" t="n">
-        <v>-0.1816091954022989</v>
+        <v>-0.232183908045977</v>
       </c>
       <c r="P108" t="n">
-        <v>-79</v>
+        <v>-101</v>
       </c>
       <c r="Q108" t="n">
-        <v>1499.666666666667</v>
+        <v>1679.666666666667</v>
       </c>
       <c r="R108" t="n">
         <v>0</v>
@@ -36073,25 +36057,25 @@
         <v>0</v>
       </c>
       <c r="D109" t="n">
-        <v>0.2507301502154942</v>
+        <v>0.2606617667228481</v>
       </c>
       <c r="E109" t="n">
-        <v>1.148577715799314</v>
+        <v>1.124828377903229</v>
       </c>
       <c r="F109" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.1633333333333333</v>
       </c>
       <c r="G109" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H109" t="n">
-        <v>1820</v>
+        <v>1821</v>
       </c>
       <c r="I109" t="n">
-        <v>0.4</v>
+        <v>0.3625</v>
       </c>
       <c r="J109" t="n">
-        <v>5.199999999999999</v>
+        <v>5.65</v>
       </c>
       <c r="K109" t="inlineStr">
         <is>
@@ -36102,25 +36086,25 @@
         <v>0</v>
       </c>
       <c r="M109" t="n">
-        <v>0.09196505739039984</v>
+        <v>0.09552887555307343</v>
       </c>
       <c r="N109" t="n">
-        <v>1.68512188856626</v>
+        <v>1.666927230292363</v>
       </c>
       <c r="O109" t="n">
-        <v>0.2183908045977012</v>
+        <v>0.2160919540229885</v>
       </c>
       <c r="P109" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q109" t="n">
-        <v>3111.666666666667</v>
+        <v>3112.666666666667</v>
       </c>
       <c r="R109" t="n">
         <v>0.3333333333333333</v>
       </c>
       <c r="S109" t="n">
-        <v>2.166666666666667</v>
+        <v>2.666666666666667</v>
       </c>
     </row>
     <row r="110">
@@ -36156,7 +36140,7 @@
         <v>1</v>
       </c>
       <c r="J110" t="n">
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="K110" t="inlineStr">
         <is>

</xml_diff>